<commit_message>
Updated CHE_grids model - 2025-08-14 22:19
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85C69D0E-C6A2-4B6B-BF39-3C79E6D75CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40A61003-E65C-4FF8-A972-882AD8243A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,16 +815,148 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0000</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_0</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0003</t>
@@ -833,298 +965,166 @@
     <t>connecting solar and wind to buses in grid cell CHE_3</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0002</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_2</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
   </si>
   <si>
     <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
   </si>
   <si>
     <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
     <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
   </si>
   <si>
     <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF0F741B-9592-B65F-65BA-DE06E6DC6FD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF28F3A2-94C6-D5B2-19A0-D8C266FACC9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18849DCD-2160-1673-F482-F9D1AB4DA896}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CC0ED89-7F58-472C-60CC-69EA42C0E1F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48093D5-AB15-3535-847C-F9E8C01711C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E767E434-9F76-D5E6-E617-7775344B2ACE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACFEBE6-49EF-76DC-3629-A89711B62024}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77DBC304-ADEE-8C46-A18E-A0808CDC6628}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BA5F30-C88B-4472-AAA2-7FC7D07EC7C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7551BCB4-D829-4FAF-BE94-9BB228E1EDF7}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BA8331-EEBC-4B63-81F4-2A1CFE1EF955}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64F45C2-0808-493F-9F23-AAEB1FA62855}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482DA79B-7C3E-4282-9052-80F0A63E7BA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B69DE62-022B-4FAC-94E9-82F7A49464C9}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-14 22:29
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40A61003-E65C-4FF8-A972-882AD8243A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1391E9A6-3E58-4B2F-9AD6-C74E660FCAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,18 +815,36 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0024</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_24</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0008</t>
   </si>
   <si>
@@ -839,6 +857,54 @@
     <t>connecting solar and wind to buses in grid cell CHE_5</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0020</t>
   </si>
   <si>
@@ -857,6 +923,18 @@
     <t>connecting solar and wind to buses in grid cell CHE_6</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0017</t>
   </si>
   <si>
@@ -875,70 +953,10 @@
     <t>connecting solar and wind to buses in grid cell CHE_23</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0014</t>
@@ -953,30 +971,30 @@
     <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
   </si>
   <si>
@@ -995,6 +1013,54 @@
     <t>e_r5378910-220,e_w161853746-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
   </si>
   <si>
@@ -1013,6 +1079,18 @@
     <t>e_w127004407-400</t>
   </si>
   <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
   </si>
   <si>
@@ -1031,70 +1109,10 @@
     <t>e_w207991759-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
@@ -1107,24 +1125,6 @@
   </si>
   <si>
     <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF28F3A2-94C6-D5B2-19A0-D8C266FACC9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F17D264-5E50-DE69-D291-F1EF8E19FF54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CC0ED89-7F58-472C-60CC-69EA42C0E1F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02FF1A7-0B49-7227-DB3B-D6303749606F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E767E434-9F76-D5E6-E617-7775344B2ACE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E957ECC-F612-591A-57B1-D83711BB66D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77DBC304-ADEE-8C46-A18E-A0808CDC6628}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7959F6A-AD9B-A5BB-E277-3B2D0F02260A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7551BCB4-D829-4FAF-BE94-9BB228E1EDF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13620E3B-38BE-4480-80DD-8A13EA67A3BD}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>188</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64F45C2-0808-493F-9F23-AAEB1FA62855}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC03E67-18D9-4439-912F-8493FF8D6601}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B69DE62-022B-4FAC-94E9-82F7A49464C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A255EC-1759-44A2-8189-C0410C97F9E6}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-14 22:36
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1391E9A6-3E58-4B2F-9AD6-C74E660FCAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A743A8-EDB3-49D0-AFA7-E1874C979349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,316 +815,316 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0012</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_12</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
   </si>
   <si>
     <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F17D264-5E50-DE69-D291-F1EF8E19FF54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6538C99-08EB-BE5F-0D60-FA6606BA6ED8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02FF1A7-0B49-7227-DB3B-D6303749606F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6061C04-74CB-C4AA-6A0D-2CB63E124A3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E957ECC-F612-591A-57B1-D83711BB66D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D16101D4-3DC8-6CD3-5972-286D5A45A902}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7959F6A-AD9B-A5BB-E277-3B2D0F02260A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE977759-B969-B448-CEE6-03091AF6CEB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13620E3B-38BE-4480-80DD-8A13EA67A3BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CE1066-D97E-46A2-801D-98AC49CFFF92}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC03E67-18D9-4439-912F-8493FF8D6601}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C01165B-92AA-4B51-8794-35FA9E23017D}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A255EC-1759-44A2-8189-C0410C97F9E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2A45AB-49D7-42E3-938C-6CA3598496BA}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-14 22:39
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A743A8-EDB3-49D0-AFA7-E1874C979349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3188C617-2056-4CED-9C3B-81A8B74DAC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,34 +815,118 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0000</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_0</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0017</t>
@@ -881,124 +965,124 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0007</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_7</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
   </si>
   <si>
     <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
@@ -1037,94 +1121,10 @@
     <t>e_r7933294-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
     <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
   </si>
   <si>
     <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6538C99-08EB-BE5F-0D60-FA6606BA6ED8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1859D984-633A-C4BF-E74B-DF6D9C050EE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6061C04-74CB-C4AA-6A0D-2CB63E124A3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE041C73-345A-72B6-1A40-7ED4487DC27D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D16101D4-3DC8-6CD3-5972-286D5A45A902}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F24D371-D6A3-E99B-6F11-A10BCE70460D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE977759-B969-B448-CEE6-03091AF6CEB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C284EC-858C-E7AB-7C4A-FD9EF6E0D3E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CE1066-D97E-46A2-801D-98AC49CFFF92}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31FD461-9353-45ED-A77C-45DC0E9C7F0D}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C01165B-92AA-4B51-8794-35FA9E23017D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047644EF-6E83-4893-8BF3-B820B383DF67}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2A45AB-49D7-42E3-938C-6CA3598496BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB6E10E-6D63-444B-98C4-632D0E560EEB}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-14 23:32
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3188C617-2056-4CED-9C3B-81A8B74DAC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A07860-8FD9-443F-A5F6-576EF772D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,18 +815,108 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0024</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_24</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0008</t>
   </si>
   <si>
@@ -839,144 +929,144 @@
     <t>connecting solar and wind to buses in grid cell CHE_5</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0003</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_3</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
   </si>
   <si>
@@ -995,136 +1085,46 @@
     <t>e_r5378910-220,e_w161853746-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
   </si>
   <si>
     <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1745,15 +1745,33 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent3 3 2" xfId="4" xr:uid="{ABC4988B-8BA7-47D0-A9D6-448C999748B6}"/>
@@ -1797,7 +1815,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>130175</xdr:colOff>
+      <xdr:colOff>296862</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
@@ -1806,7 +1824,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1859D984-633A-C4BF-E74B-DF6D9C050EE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B7E0FC-5A66-DDAD-695E-36E44C3778D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1879,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE041C73-345A-72B6-1A40-7ED4487DC27D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D021E6FC-D259-94D6-DE53-45FD00B523A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1934,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F24D371-D6A3-E99B-6F11-A10BCE70460D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DCD9A89-8AC3-0D89-F21A-F4CB3378AB8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1989,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C284EC-858C-E7AB-7C4A-FD9EF6E0D3E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0FE391-D573-517E-7CF2-7EF61A19AA37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2776,17 +2794,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="3" max="3" width="12.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.59765625" customWidth="1"/>
-    <col min="5" max="6" width="10.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" customWidth="1"/>
-    <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.59765625" customWidth="1"/>
+    <col min="2" max="7" width="10.59765625" customWidth="1"/>
+    <col min="9" max="14" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.05" customHeight="1">
@@ -2809,7 +2818,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+    <row r="3" spans="1:14" ht="31.15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>6</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="52.5">
       <c r="B4" s="30" t="s">
         <v>17</v>
       </c>
@@ -2881,7 +2890,7 @@
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" ht="52.5">
       <c r="B5" s="31" t="s">
         <v>17</v>
       </c>
@@ -2915,7 +2924,7 @@
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" ht="52.5">
       <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
@@ -4474,7 +4483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31FD461-9353-45ED-A77C-45DC0E9C7F0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E460B43-C2E9-4134-B546-D8214582C8FB}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4483,28 +4492,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.59765625" customWidth="1"/>
-    <col min="18" max="18" width="10.59765625" customWidth="1"/>
-    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.59765625" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.59765625" customWidth="1"/>
-    <col min="24" max="24" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.59765625" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.53125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.59765625" customWidth="1"/>
+    <col min="2" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="15" width="10.59765625" customWidth="1"/>
+    <col min="18" max="25" width="10.59765625" customWidth="1"/>
+    <col min="29" max="30" width="10.59765625" customWidth="1"/>
+    <col min="31" max="31" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4534,7 +4526,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15.75" thickBot="1">
+    <row r="3" spans="1:33" ht="31.15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>123</v>
       </c>
@@ -4611,7 +4603,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" ht="157.5">
       <c r="B4" s="30" t="s">
         <v>127</v>
       </c>
@@ -4685,10 +4677,10 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="183.75">
       <c r="B5" s="31" t="s">
         <v>127</v>
       </c>
@@ -4762,10 +4754,10 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="65.650000000000006">
       <c r="B6" s="30" t="s">
         <v>127</v>
       </c>
@@ -4839,10 +4831,10 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="157.5">
       <c r="B7" s="31" t="s">
         <v>127</v>
       </c>
@@ -4916,10 +4908,10 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="275.64999999999998">
       <c r="B8" s="30" t="s">
         <v>127</v>
       </c>
@@ -4993,10 +4985,10 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="118.15">
       <c r="B9" s="31" t="s">
         <v>127</v>
       </c>
@@ -5070,10 +5062,10 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="393.75">
       <c r="B10" s="30" t="s">
         <v>127</v>
       </c>
@@ -5147,10 +5139,10 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="249.4">
       <c r="B11" s="31" t="s">
         <v>127</v>
       </c>
@@ -5224,10 +5216,10 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="170.65">
       <c r="B12" s="30" t="s">
         <v>127</v>
       </c>
@@ -5301,10 +5293,10 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="65.650000000000006">
       <c r="B13" s="31" t="s">
         <v>127</v>
       </c>
@@ -5378,10 +5370,10 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="65.650000000000006">
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
@@ -5455,10 +5447,10 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="157.5">
       <c r="B15" s="31" t="s">
         <v>127</v>
       </c>
@@ -5532,10 +5524,10 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="65.650000000000006">
       <c r="B16" s="30" t="s">
         <v>127</v>
       </c>
@@ -5609,10 +5601,10 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="17" spans="2:33">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="2:33" ht="118.15">
       <c r="B17" s="31" t="s">
         <v>127</v>
       </c>
@@ -5686,10 +5678,10 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="2:33">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="2:33" ht="170.65">
       <c r="B18" s="30" t="s">
         <v>127</v>
       </c>
@@ -5763,10 +5755,10 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="19" spans="2:33">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="2:33" ht="65.650000000000006">
       <c r="B19" s="31" t="s">
         <v>127</v>
       </c>
@@ -5840,10 +5832,10 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="2:33">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="2:33" ht="105">
       <c r="B20" s="30" t="s">
         <v>127</v>
       </c>
@@ -5917,10 +5909,10 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="2:33">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="2:33" ht="65.650000000000006">
       <c r="B21" s="31" t="s">
         <v>127</v>
       </c>
@@ -5994,10 +5986,10 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="2:33">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="2:33" ht="288.75">
       <c r="B22" s="30" t="s">
         <v>127</v>
       </c>
@@ -6071,10 +6063,10 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="2:33">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="2:33" ht="105">
       <c r="B23" s="31" t="s">
         <v>127</v>
       </c>
@@ -6148,10 +6140,10 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="2:33">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="2:33" ht="65.650000000000006">
       <c r="B24" s="30" t="s">
         <v>127</v>
       </c>
@@ -6225,10 +6217,10 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="2:33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="2:33" ht="65.650000000000006">
       <c r="B25" s="31" t="s">
         <v>127</v>
       </c>
@@ -6302,10 +6294,10 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="2:33">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33" ht="223.15">
       <c r="B26" s="30" t="s">
         <v>127</v>
       </c>
@@ -6379,10 +6371,10 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="2:33">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33" ht="105">
       <c r="B27" s="31" t="s">
         <v>127</v>
       </c>
@@ -6456,10 +6448,10 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="2:33">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="2:33" ht="288.75">
       <c r="B28" s="30" t="s">
         <v>127</v>
       </c>
@@ -6533,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047644EF-6E83-4893-8BF3-B820B383DF67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8E5D4D-A76A-4690-94B5-107F0CEFFA52}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6555,17 +6547,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.59765625" customWidth="1"/>
+    <col min="2" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="15" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.05" customHeight="1">
@@ -6588,7 +6571,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1">
+    <row r="3" spans="1:15" ht="31.15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>123</v>
       </c>
@@ -6626,7 +6609,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="52.5">
       <c r="B4" s="30" t="s">
         <v>127</v>
       </c>
@@ -6664,7 +6647,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" ht="52.5">
       <c r="B5" s="31" t="s">
         <v>127</v>
       </c>
@@ -6702,7 +6685,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="52.5">
       <c r="B6" s="30" t="s">
         <v>127</v>
       </c>
@@ -6740,7 +6723,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="52.5">
       <c r="B7" s="31" t="s">
         <v>127</v>
       </c>
@@ -6778,7 +6761,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="52.5">
       <c r="B8" s="30" t="s">
         <v>127</v>
       </c>
@@ -6816,7 +6799,7 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="52.5">
       <c r="B9" s="31" t="s">
         <v>127</v>
       </c>
@@ -6854,7 +6837,7 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="52.5">
       <c r="B10" s="30" t="s">
         <v>127</v>
       </c>
@@ -6892,7 +6875,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="52.5">
       <c r="B11" s="31" t="s">
         <v>127</v>
       </c>
@@ -6930,7 +6913,7 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="52.5">
       <c r="B12" s="30" t="s">
         <v>127</v>
       </c>
@@ -6968,7 +6951,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="52.5">
       <c r="B13" s="31" t="s">
         <v>127</v>
       </c>
@@ -7006,7 +6989,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="52.5">
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
@@ -7044,7 +7027,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" ht="52.5">
       <c r="B15" s="31" t="s">
         <v>127</v>
       </c>
@@ -7082,7 +7065,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" ht="52.5">
       <c r="B16" s="30" t="s">
         <v>127</v>
       </c>
@@ -7120,7 +7103,7 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" ht="52.5">
       <c r="B17" s="31" t="s">
         <v>127</v>
       </c>
@@ -7158,7 +7141,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" ht="52.5">
       <c r="B18" s="30" t="s">
         <v>127</v>
       </c>
@@ -7196,7 +7179,7 @@
         <v>0.156</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" ht="52.5">
       <c r="B19" s="31" t="s">
         <v>127</v>
       </c>
@@ -7234,7 +7217,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" ht="52.5">
       <c r="B20" s="30" t="s">
         <v>127</v>
       </c>
@@ -7272,7 +7255,7 @@
         <v>0.156</v>
       </c>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" ht="52.5">
       <c r="B21" s="31" t="s">
         <v>127</v>
       </c>
@@ -7310,7 +7293,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" ht="52.5">
       <c r="B22" s="30" t="s">
         <v>127</v>
       </c>
@@ -7348,7 +7331,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" ht="52.5">
       <c r="B23" s="31" t="s">
         <v>127</v>
       </c>
@@ -7386,7 +7369,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" ht="52.5">
       <c r="B24" s="30" t="s">
         <v>127</v>
       </c>
@@ -7424,7 +7407,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" ht="52.5">
       <c r="B25" s="31" t="s">
         <v>127</v>
       </c>
@@ -7462,7 +7445,7 @@
         <v>0.219</v>
       </c>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" ht="52.5">
       <c r="B26" s="30" t="s">
         <v>127</v>
       </c>
@@ -7500,7 +7483,7 @@
         <v>0.223</v>
       </c>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" ht="52.5">
       <c r="B27" s="31" t="s">
         <v>127</v>
       </c>
@@ -7538,7 +7521,7 @@
         <v>0.183</v>
       </c>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" ht="52.5">
       <c r="B28" s="30" t="s">
         <v>127</v>
       </c>
@@ -7576,7 +7559,7 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" ht="52.5">
       <c r="B29" s="31" t="s">
         <v>127</v>
       </c>
@@ -7624,22 +7607,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB6E10E-6D63-444B-98C4-632D0E560EEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D4B206-7B81-40BB-969B-8F548C831770}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="30.59765625" customWidth="1"/>
-    <col min="3" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="30.59765625" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.59765625" customWidth="1"/>
+    <col min="2" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="17" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.05" customHeight="1">
@@ -7662,7 +7638,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:17" ht="31.15" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>108</v>
       </c>
@@ -7706,7 +7682,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" ht="26.25">
       <c r="B4" s="30" t="s">
         <v>419</v>
       </c>
@@ -7748,7 +7724,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" ht="39.4">
       <c r="B5" s="31" t="s">
         <v>419</v>
       </c>
@@ -7790,7 +7766,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" ht="26.25">
       <c r="B6" s="30" t="s">
         <v>419</v>
       </c>
@@ -7832,7 +7808,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" ht="26.25">
       <c r="B7" s="31" t="s">
         <v>419</v>
       </c>
@@ -7874,7 +7850,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" ht="26.25">
       <c r="B8" s="30" t="s">
         <v>419</v>
       </c>
@@ -7916,7 +7892,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" ht="52.5">
       <c r="B9" s="31" t="s">
         <v>424</v>
       </c>
@@ -7958,7 +7934,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" ht="39.4">
       <c r="B10" s="30" t="s">
         <v>424</v>
       </c>
@@ -8000,7 +7976,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" ht="39.4">
       <c r="B11" s="31" t="s">
         <v>424</v>
       </c>
@@ -8042,7 +8018,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" ht="39.4">
       <c r="B12" s="30" t="s">
         <v>424</v>
       </c>
@@ -8084,7 +8060,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" ht="39.4">
       <c r="B13" s="31" t="s">
         <v>424</v>
       </c>
@@ -8168,7 +8144,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" ht="26.25">
       <c r="B15" s="31" t="s">
         <v>425</v>
       </c>
@@ -8210,7 +8186,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" ht="52.5">
       <c r="B16" s="30" t="s">
         <v>425</v>
       </c>
@@ -8252,7 +8228,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:17" ht="26.25">
       <c r="B17" s="31" t="s">
         <v>426</v>
       </c>
@@ -8294,7 +8270,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:17" ht="39.4">
       <c r="B18" s="30" t="s">
         <v>426</v>
       </c>
@@ -8336,7 +8312,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" ht="39.4">
       <c r="B19" s="31" t="s">
         <v>426</v>
       </c>
@@ -8378,7 +8354,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:17" ht="26.25">
       <c r="B20" s="30" t="s">
         <v>427</v>
       </c>
@@ -8420,7 +8396,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" ht="26.25">
       <c r="B21" s="31" t="s">
         <v>427</v>
       </c>
@@ -8485,7 +8461,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" ht="52.5">
       <c r="B23" s="31" t="s">
         <v>428</v>
       </c>
@@ -8508,7 +8484,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" ht="52.5">
       <c r="B24" s="30" t="s">
         <v>428</v>
       </c>
@@ -8531,7 +8507,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" ht="52.5">
       <c r="B25" s="31" t="s">
         <v>428</v>
       </c>
@@ -8623,7 +8599,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="2:17">
+    <row r="29" spans="2:17" ht="39.4">
       <c r="B29" s="31" t="s">
         <v>430</v>
       </c>
@@ -8646,7 +8622,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="2:17">
+    <row r="30" spans="2:17" ht="39.4">
       <c r="B30" s="30" t="s">
         <v>430</v>
       </c>
@@ -8669,7 +8645,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" ht="39.4">
       <c r="B31" s="31" t="s">
         <v>430</v>
       </c>
@@ -8692,7 +8668,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" ht="39.4">
       <c r="B32" s="30" t="s">
         <v>430</v>
       </c>
@@ -8715,7 +8691,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" ht="39.4">
       <c r="B33" s="31" t="s">
         <v>430</v>
       </c>
@@ -8945,7 +8921,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" ht="26.25">
       <c r="B43" s="31" t="s">
         <v>434</v>
       </c>
@@ -8968,7 +8944,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" ht="26.25">
       <c r="B44" s="30" t="s">
         <v>434</v>
       </c>
@@ -8991,7 +8967,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" ht="26.25">
       <c r="B45" s="31" t="s">
         <v>434</v>
       </c>
@@ -9014,7 +8990,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" ht="52.5">
       <c r="B46" s="30" t="s">
         <v>435</v>
       </c>
@@ -9037,7 +9013,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" ht="52.5">
       <c r="B47" s="31" t="s">
         <v>435</v>
       </c>
@@ -9060,7 +9036,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" ht="52.5">
       <c r="B48" s="30" t="s">
         <v>435</v>
       </c>
@@ -9083,7 +9059,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:8" ht="52.5">
       <c r="B49" s="31" t="s">
         <v>435</v>
       </c>
@@ -9106,7 +9082,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="2:8">
+    <row r="50" spans="2:8" ht="52.5">
       <c r="B50" s="30" t="s">
         <v>435</v>
       </c>
@@ -9129,7 +9105,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="2:8" ht="26.25">
       <c r="B51" s="31" t="s">
         <v>436</v>
       </c>
@@ -9152,7 +9128,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:8" ht="26.25">
       <c r="B52" s="30" t="s">
         <v>436</v>
       </c>
@@ -9175,7 +9151,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="53" spans="2:8">
+    <row r="53" spans="2:8" ht="26.25">
       <c r="B53" s="31" t="s">
         <v>436</v>
       </c>
@@ -9198,7 +9174,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="54" spans="2:8">
+    <row r="54" spans="2:8" ht="39.4">
       <c r="B54" s="30" t="s">
         <v>437</v>
       </c>
@@ -9221,7 +9197,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="2:8">
+    <row r="55" spans="2:8" ht="39.4">
       <c r="B55" s="31" t="s">
         <v>437</v>
       </c>
@@ -9244,7 +9220,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="56" spans="2:8">
+    <row r="56" spans="2:8" ht="39.4">
       <c r="B56" s="30" t="s">
         <v>437</v>
       </c>
@@ -9267,7 +9243,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="57" spans="2:8">
+    <row r="57" spans="2:8" ht="39.4">
       <c r="B57" s="31" t="s">
         <v>438</v>
       </c>
@@ -9290,7 +9266,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="58" spans="2:8">
+    <row r="58" spans="2:8" ht="39.4">
       <c r="B58" s="30" t="s">
         <v>438</v>
       </c>
@@ -9313,7 +9289,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="2:8">
+    <row r="59" spans="2:8" ht="39.4">
       <c r="B59" s="31" t="s">
         <v>438</v>
       </c>
@@ -9336,7 +9312,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="60" spans="2:8">
+    <row r="60" spans="2:8" ht="26.25">
       <c r="B60" s="30" t="s">
         <v>439</v>
       </c>
@@ -9359,7 +9335,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="61" spans="2:8">
+    <row r="61" spans="2:8" ht="26.25">
       <c r="B61" s="31" t="s">
         <v>439</v>
       </c>
@@ -9382,7 +9358,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="62" spans="2:8">
+    <row r="62" spans="2:8" ht="26.25">
       <c r="B62" s="30" t="s">
         <v>439</v>
       </c>
@@ -9405,7 +9381,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="63" spans="2:8">
+    <row r="63" spans="2:8" ht="26.25">
       <c r="B63" s="31" t="s">
         <v>439</v>
       </c>
@@ -9428,7 +9404,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="64" spans="2:8">
+    <row r="64" spans="2:8" ht="26.25">
       <c r="B64" s="30" t="s">
         <v>439</v>
       </c>
@@ -9451,7 +9427,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="65" spans="2:8">
+    <row r="65" spans="2:8" ht="26.25">
       <c r="B65" s="31" t="s">
         <v>440</v>
       </c>
@@ -9474,7 +9450,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="66" spans="2:8">
+    <row r="66" spans="2:8" ht="26.25">
       <c r="B66" s="30" t="s">
         <v>440</v>
       </c>
@@ -9497,7 +9473,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="67" spans="2:8">
+    <row r="67" spans="2:8" ht="26.25">
       <c r="B67" s="31" t="s">
         <v>440</v>
       </c>
@@ -9520,7 +9496,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="68" spans="2:8">
+    <row r="68" spans="2:8" ht="26.25">
       <c r="B68" s="30" t="s">
         <v>440</v>
       </c>
@@ -9543,7 +9519,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="69" spans="2:8">
+    <row r="69" spans="2:8" ht="26.25">
       <c r="B69" s="31" t="s">
         <v>440</v>
       </c>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 00:41
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A07860-8FD9-443F-A5F6-576EF772D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC66A40B-F00C-4F78-A3F9-4A3F9B2BCA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,18 +815,72 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0011</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_11</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0015</t>
   </si>
   <si>
@@ -839,10 +893,52 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0012</t>
@@ -851,84 +947,6 @@
     <t>connecting solar and wind to buses in grid cell CHE_12</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0020</t>
   </si>
   <si>
@@ -947,24 +965,6 @@
     <t>connecting solar and wind to buses in grid cell CHE_6</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0003</t>
   </si>
   <si>
@@ -977,6 +977,60 @@
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
   </si>
   <si>
@@ -995,10 +1049,52 @@
     <t>e_r7933294-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
   </si>
   <si>
     <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
@@ -1007,84 +1103,6 @@
     <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
     <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
   </si>
   <si>
@@ -1101,24 +1119,6 @@
   </si>
   <si>
     <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
@@ -1745,33 +1745,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent3 3 2" xfId="4" xr:uid="{ABC4988B-8BA7-47D0-A9D6-448C999748B6}"/>
@@ -1815,7 +1797,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>296862</xdr:colOff>
+      <xdr:colOff>130175</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
@@ -1824,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B7E0FC-5A66-DDAD-695E-36E44C3778D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E1BB19-49DC-C8BD-5D36-F42D3E7EAD4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1879,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D021E6FC-D259-94D6-DE53-45FD00B523A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F327D75E-7FFF-0A86-DDD9-1C78100700B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DCD9A89-8AC3-0D89-F21A-F4CB3378AB8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2E4B65-4CFF-DE42-F1FB-42EEFAD01E14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1989,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0FE391-D573-517E-7CF2-7EF61A19AA37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91902494-60A6-4EDF-BB5E-BC798EBF2CCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2794,8 +2776,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="7" width="10.59765625" customWidth="1"/>
-    <col min="9" max="14" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.59765625" customWidth="1"/>
+    <col min="5" max="6" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.05" customHeight="1">
@@ -2818,7 +2809,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="31.15" thickBot="1">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>6</v>
       </c>
@@ -2856,7 +2847,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="52.5">
+    <row r="4" spans="1:14">
       <c r="B4" s="30" t="s">
         <v>17</v>
       </c>
@@ -2890,7 +2881,7 @@
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
     </row>
-    <row r="5" spans="1:14" ht="52.5">
+    <row r="5" spans="1:14">
       <c r="B5" s="31" t="s">
         <v>17</v>
       </c>
@@ -2924,7 +2915,7 @@
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
     </row>
-    <row r="6" spans="1:14" ht="52.5">
+    <row r="6" spans="1:14">
       <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
@@ -4483,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E460B43-C2E9-4134-B546-D8214582C8FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AFF12E-A44F-4DD2-A4D8-F4648BC95315}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4492,11 +4483,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="15" width="10.59765625" customWidth="1"/>
-    <col min="18" max="25" width="10.59765625" customWidth="1"/>
-    <col min="29" max="30" width="10.59765625" customWidth="1"/>
-    <col min="31" max="31" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.59765625" customWidth="1"/>
+    <col min="18" max="18" width="10.59765625" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.59765625" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.59765625" customWidth="1"/>
+    <col min="24" max="24" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.59765625" customWidth="1"/>
+    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.59765625" customWidth="1"/>
     <col min="32" max="33" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4526,7 +4534,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="31.15" thickBot="1">
+    <row r="3" spans="1:33" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>123</v>
       </c>
@@ -4603,7 +4611,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="157.5">
+    <row r="4" spans="1:33">
       <c r="B4" s="30" t="s">
         <v>127</v>
       </c>
@@ -4677,10 +4685,10 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" ht="183.75">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="B5" s="31" t="s">
         <v>127</v>
       </c>
@@ -4754,10 +4762,10 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="65.650000000000006">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
       <c r="B6" s="30" t="s">
         <v>127</v>
       </c>
@@ -4831,10 +4839,10 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="157.5">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
       <c r="B7" s="31" t="s">
         <v>127</v>
       </c>
@@ -4908,10 +4916,10 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="275.64999999999998">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
       <c r="B8" s="30" t="s">
         <v>127</v>
       </c>
@@ -4985,10 +4993,10 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" ht="118.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
       <c r="B9" s="31" t="s">
         <v>127</v>
       </c>
@@ -5065,7 +5073,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="393.75">
+    <row r="10" spans="1:33">
       <c r="B10" s="30" t="s">
         <v>127</v>
       </c>
@@ -5139,10 +5147,10 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" ht="249.4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
       <c r="B11" s="31" t="s">
         <v>127</v>
       </c>
@@ -5216,10 +5224,10 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" ht="170.65">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
       <c r="B12" s="30" t="s">
         <v>127</v>
       </c>
@@ -5293,10 +5301,10 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" ht="65.650000000000006">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
       <c r="B13" s="31" t="s">
         <v>127</v>
       </c>
@@ -5370,10 +5378,10 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="65.650000000000006">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
@@ -5447,10 +5455,10 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" ht="157.5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
       <c r="B15" s="31" t="s">
         <v>127</v>
       </c>
@@ -5524,10 +5532,10 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="65.650000000000006">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
       <c r="B16" s="30" t="s">
         <v>127</v>
       </c>
@@ -5601,10 +5609,10 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="2:33" ht="118.15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="2:33">
       <c r="B17" s="31" t="s">
         <v>127</v>
       </c>
@@ -5678,10 +5686,10 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="2:33" ht="170.65">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="2:33">
       <c r="B18" s="30" t="s">
         <v>127</v>
       </c>
@@ -5758,7 +5766,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="65.650000000000006">
+    <row r="19" spans="2:33">
       <c r="B19" s="31" t="s">
         <v>127</v>
       </c>
@@ -5832,10 +5840,10 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="2:33" ht="105">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="2:33">
       <c r="B20" s="30" t="s">
         <v>127</v>
       </c>
@@ -5909,10 +5917,10 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="2:33" ht="65.650000000000006">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:33">
       <c r="B21" s="31" t="s">
         <v>127</v>
       </c>
@@ -5986,10 +5994,10 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="22" spans="2:33" ht="288.75">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="2:33">
       <c r="B22" s="30" t="s">
         <v>127</v>
       </c>
@@ -6063,10 +6071,10 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="2:33" ht="105">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="2:33">
       <c r="B23" s="31" t="s">
         <v>127</v>
       </c>
@@ -6140,10 +6148,10 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="2:33" ht="65.650000000000006">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="2:33">
       <c r="B24" s="30" t="s">
         <v>127</v>
       </c>
@@ -6217,10 +6225,10 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="2:33" ht="65.650000000000006">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="2:33">
       <c r="B25" s="31" t="s">
         <v>127</v>
       </c>
@@ -6294,10 +6302,10 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="2:33" ht="223.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33">
       <c r="B26" s="30" t="s">
         <v>127</v>
       </c>
@@ -6371,10 +6379,10 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="2:33" ht="105">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33">
       <c r="B27" s="31" t="s">
         <v>127</v>
       </c>
@@ -6448,10 +6456,10 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="2:33" ht="288.75">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="2:33">
       <c r="B28" s="30" t="s">
         <v>127</v>
       </c>
@@ -6538,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8E5D4D-A76A-4690-94B5-107F0CEFFA52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF16765-DA2B-4117-8983-5F76C938EF76}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6547,8 +6555,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="15" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.05" customHeight="1">
@@ -6571,7 +6588,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="31.15" thickBot="1">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>123</v>
       </c>
@@ -6609,7 +6626,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="52.5">
+    <row r="4" spans="1:15">
       <c r="B4" s="30" t="s">
         <v>127</v>
       </c>
@@ -6647,7 +6664,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="52.5">
+    <row r="5" spans="1:15">
       <c r="B5" s="31" t="s">
         <v>127</v>
       </c>
@@ -6685,7 +6702,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="52.5">
+    <row r="6" spans="1:15">
       <c r="B6" s="30" t="s">
         <v>127</v>
       </c>
@@ -6723,7 +6740,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="52.5">
+    <row r="7" spans="1:15">
       <c r="B7" s="31" t="s">
         <v>127</v>
       </c>
@@ -6761,7 +6778,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="52.5">
+    <row r="8" spans="1:15">
       <c r="B8" s="30" t="s">
         <v>127</v>
       </c>
@@ -6799,7 +6816,7 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="52.5">
+    <row r="9" spans="1:15">
       <c r="B9" s="31" t="s">
         <v>127</v>
       </c>
@@ -6837,7 +6854,7 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="52.5">
+    <row r="10" spans="1:15">
       <c r="B10" s="30" t="s">
         <v>127</v>
       </c>
@@ -6875,7 +6892,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="52.5">
+    <row r="11" spans="1:15">
       <c r="B11" s="31" t="s">
         <v>127</v>
       </c>
@@ -6913,7 +6930,7 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="52.5">
+    <row r="12" spans="1:15">
       <c r="B12" s="30" t="s">
         <v>127</v>
       </c>
@@ -6951,7 +6968,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="52.5">
+    <row r="13" spans="1:15">
       <c r="B13" s="31" t="s">
         <v>127</v>
       </c>
@@ -6989,7 +7006,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="52.5">
+    <row r="14" spans="1:15">
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
@@ -7027,7 +7044,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="52.5">
+    <row r="15" spans="1:15">
       <c r="B15" s="31" t="s">
         <v>127</v>
       </c>
@@ -7065,7 +7082,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="52.5">
+    <row r="16" spans="1:15">
       <c r="B16" s="30" t="s">
         <v>127</v>
       </c>
@@ -7103,7 +7120,7 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="52.5">
+    <row r="17" spans="2:15">
       <c r="B17" s="31" t="s">
         <v>127</v>
       </c>
@@ -7141,7 +7158,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="52.5">
+    <row r="18" spans="2:15">
       <c r="B18" s="30" t="s">
         <v>127</v>
       </c>
@@ -7179,7 +7196,7 @@
         <v>0.156</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="52.5">
+    <row r="19" spans="2:15">
       <c r="B19" s="31" t="s">
         <v>127</v>
       </c>
@@ -7217,7 +7234,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="52.5">
+    <row r="20" spans="2:15">
       <c r="B20" s="30" t="s">
         <v>127</v>
       </c>
@@ -7255,7 +7272,7 @@
         <v>0.156</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="52.5">
+    <row r="21" spans="2:15">
       <c r="B21" s="31" t="s">
         <v>127</v>
       </c>
@@ -7293,7 +7310,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="52.5">
+    <row r="22" spans="2:15">
       <c r="B22" s="30" t="s">
         <v>127</v>
       </c>
@@ -7331,7 +7348,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="52.5">
+    <row r="23" spans="2:15">
       <c r="B23" s="31" t="s">
         <v>127</v>
       </c>
@@ -7369,7 +7386,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="52.5">
+    <row r="24" spans="2:15">
       <c r="B24" s="30" t="s">
         <v>127</v>
       </c>
@@ -7407,7 +7424,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="52.5">
+    <row r="25" spans="2:15">
       <c r="B25" s="31" t="s">
         <v>127</v>
       </c>
@@ -7445,7 +7462,7 @@
         <v>0.219</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="52.5">
+    <row r="26" spans="2:15">
       <c r="B26" s="30" t="s">
         <v>127</v>
       </c>
@@ -7483,7 +7500,7 @@
         <v>0.223</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="52.5">
+    <row r="27" spans="2:15">
       <c r="B27" s="31" t="s">
         <v>127</v>
       </c>
@@ -7521,7 +7538,7 @@
         <v>0.183</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="52.5">
+    <row r="28" spans="2:15">
       <c r="B28" s="30" t="s">
         <v>127</v>
       </c>
@@ -7559,7 +7576,7 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:15" ht="52.5">
+    <row r="29" spans="2:15">
       <c r="B29" s="31" t="s">
         <v>127</v>
       </c>
@@ -7607,15 +7624,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D4B206-7B81-40BB-969B-8F548C831770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770D557E-9C91-46EF-B281-7F4D115EC9EF}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="8" width="10.59765625" customWidth="1"/>
-    <col min="11" max="17" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="30.59765625" customWidth="1"/>
+    <col min="13" max="13" width="10.59765625" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.05" customHeight="1">
@@ -7638,7 +7662,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="31.15" thickBot="1">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>108</v>
       </c>
@@ -7682,7 +7706,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="26.25">
+    <row r="4" spans="1:17">
       <c r="B4" s="30" t="s">
         <v>419</v>
       </c>
@@ -7724,7 +7748,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="39.4">
+    <row r="5" spans="1:17">
       <c r="B5" s="31" t="s">
         <v>419</v>
       </c>
@@ -7766,7 +7790,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="26.25">
+    <row r="6" spans="1:17">
       <c r="B6" s="30" t="s">
         <v>419</v>
       </c>
@@ -7808,7 +7832,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="26.25">
+    <row r="7" spans="1:17">
       <c r="B7" s="31" t="s">
         <v>419</v>
       </c>
@@ -7850,7 +7874,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="26.25">
+    <row r="8" spans="1:17">
       <c r="B8" s="30" t="s">
         <v>419</v>
       </c>
@@ -7892,7 +7916,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="52.5">
+    <row r="9" spans="1:17">
       <c r="B9" s="31" t="s">
         <v>424</v>
       </c>
@@ -7934,7 +7958,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="39.4">
+    <row r="10" spans="1:17">
       <c r="B10" s="30" t="s">
         <v>424</v>
       </c>
@@ -7976,7 +8000,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="39.4">
+    <row r="11" spans="1:17">
       <c r="B11" s="31" t="s">
         <v>424</v>
       </c>
@@ -8018,7 +8042,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="39.4">
+    <row r="12" spans="1:17">
       <c r="B12" s="30" t="s">
         <v>424</v>
       </c>
@@ -8060,7 +8084,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="39.4">
+    <row r="13" spans="1:17">
       <c r="B13" s="31" t="s">
         <v>424</v>
       </c>
@@ -8144,7 +8168,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="26.25">
+    <row r="15" spans="1:17">
       <c r="B15" s="31" t="s">
         <v>425</v>
       </c>
@@ -8186,7 +8210,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="52.5">
+    <row r="16" spans="1:17">
       <c r="B16" s="30" t="s">
         <v>425</v>
       </c>
@@ -8228,7 +8252,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="26.25">
+    <row r="17" spans="2:17">
       <c r="B17" s="31" t="s">
         <v>426</v>
       </c>
@@ -8270,7 +8294,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="39.4">
+    <row r="18" spans="2:17">
       <c r="B18" s="30" t="s">
         <v>426</v>
       </c>
@@ -8312,7 +8336,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="39.4">
+    <row r="19" spans="2:17">
       <c r="B19" s="31" t="s">
         <v>426</v>
       </c>
@@ -8354,7 +8378,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="26.25">
+    <row r="20" spans="2:17">
       <c r="B20" s="30" t="s">
         <v>427</v>
       </c>
@@ -8396,7 +8420,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="26.25">
+    <row r="21" spans="2:17">
       <c r="B21" s="31" t="s">
         <v>427</v>
       </c>
@@ -8461,7 +8485,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="52.5">
+    <row r="23" spans="2:17">
       <c r="B23" s="31" t="s">
         <v>428</v>
       </c>
@@ -8484,7 +8508,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="52.5">
+    <row r="24" spans="2:17">
       <c r="B24" s="30" t="s">
         <v>428</v>
       </c>
@@ -8507,7 +8531,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="52.5">
+    <row r="25" spans="2:17">
       <c r="B25" s="31" t="s">
         <v>428</v>
       </c>
@@ -8599,7 +8623,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="39.4">
+    <row r="29" spans="2:17">
       <c r="B29" s="31" t="s">
         <v>430</v>
       </c>
@@ -8622,7 +8646,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="39.4">
+    <row r="30" spans="2:17">
       <c r="B30" s="30" t="s">
         <v>430</v>
       </c>
@@ -8645,7 +8669,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="39.4">
+    <row r="31" spans="2:17">
       <c r="B31" s="31" t="s">
         <v>430</v>
       </c>
@@ -8668,7 +8692,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="39.4">
+    <row r="32" spans="2:17">
       <c r="B32" s="30" t="s">
         <v>430</v>
       </c>
@@ -8691,7 +8715,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="39.4">
+    <row r="33" spans="2:8">
       <c r="B33" s="31" t="s">
         <v>430</v>
       </c>
@@ -8921,7 +8945,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="26.25">
+    <row r="43" spans="2:8">
       <c r="B43" s="31" t="s">
         <v>434</v>
       </c>
@@ -8944,7 +8968,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="26.25">
+    <row r="44" spans="2:8">
       <c r="B44" s="30" t="s">
         <v>434</v>
       </c>
@@ -8967,7 +8991,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="26.25">
+    <row r="45" spans="2:8">
       <c r="B45" s="31" t="s">
         <v>434</v>
       </c>
@@ -8990,7 +9014,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="52.5">
+    <row r="46" spans="2:8">
       <c r="B46" s="30" t="s">
         <v>435</v>
       </c>
@@ -9013,7 +9037,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="52.5">
+    <row r="47" spans="2:8">
       <c r="B47" s="31" t="s">
         <v>435</v>
       </c>
@@ -9036,7 +9060,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="52.5">
+    <row r="48" spans="2:8">
       <c r="B48" s="30" t="s">
         <v>435</v>
       </c>
@@ -9059,7 +9083,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="52.5">
+    <row r="49" spans="2:8">
       <c r="B49" s="31" t="s">
         <v>435</v>
       </c>
@@ -9082,7 +9106,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="52.5">
+    <row r="50" spans="2:8">
       <c r="B50" s="30" t="s">
         <v>435</v>
       </c>
@@ -9105,7 +9129,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="26.25">
+    <row r="51" spans="2:8">
       <c r="B51" s="31" t="s">
         <v>436</v>
       </c>
@@ -9128,7 +9152,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="26.25">
+    <row r="52" spans="2:8">
       <c r="B52" s="30" t="s">
         <v>436</v>
       </c>
@@ -9151,7 +9175,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="26.25">
+    <row r="53" spans="2:8">
       <c r="B53" s="31" t="s">
         <v>436</v>
       </c>
@@ -9174,7 +9198,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="39.4">
+    <row r="54" spans="2:8">
       <c r="B54" s="30" t="s">
         <v>437</v>
       </c>
@@ -9197,7 +9221,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="39.4">
+    <row r="55" spans="2:8">
       <c r="B55" s="31" t="s">
         <v>437</v>
       </c>
@@ -9220,7 +9244,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="39.4">
+    <row r="56" spans="2:8">
       <c r="B56" s="30" t="s">
         <v>437</v>
       </c>
@@ -9243,7 +9267,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="39.4">
+    <row r="57" spans="2:8">
       <c r="B57" s="31" t="s">
         <v>438</v>
       </c>
@@ -9266,7 +9290,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="39.4">
+    <row r="58" spans="2:8">
       <c r="B58" s="30" t="s">
         <v>438</v>
       </c>
@@ -9289,7 +9313,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="39.4">
+    <row r="59" spans="2:8">
       <c r="B59" s="31" t="s">
         <v>438</v>
       </c>
@@ -9312,7 +9336,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="26.25">
+    <row r="60" spans="2:8">
       <c r="B60" s="30" t="s">
         <v>439</v>
       </c>
@@ -9335,7 +9359,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="26.25">
+    <row r="61" spans="2:8">
       <c r="B61" s="31" t="s">
         <v>439</v>
       </c>
@@ -9358,7 +9382,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="26.25">
+    <row r="62" spans="2:8">
       <c r="B62" s="30" t="s">
         <v>439</v>
       </c>
@@ -9381,7 +9405,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="26.25">
+    <row r="63" spans="2:8">
       <c r="B63" s="31" t="s">
         <v>439</v>
       </c>
@@ -9404,7 +9428,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="26.25">
+    <row r="64" spans="2:8">
       <c r="B64" s="30" t="s">
         <v>439</v>
       </c>
@@ -9427,7 +9451,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="26.25">
+    <row r="65" spans="2:8">
       <c r="B65" s="31" t="s">
         <v>440</v>
       </c>
@@ -9450,7 +9474,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="26.25">
+    <row r="66" spans="2:8">
       <c r="B66" s="30" t="s">
         <v>440</v>
       </c>
@@ -9473,7 +9497,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="26.25">
+    <row r="67" spans="2:8">
       <c r="B67" s="31" t="s">
         <v>440</v>
       </c>
@@ -9496,7 +9520,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="26.25">
+    <row r="68" spans="2:8">
       <c r="B68" s="30" t="s">
         <v>440</v>
       </c>
@@ -9519,7 +9543,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="26.25">
+    <row r="69" spans="2:8">
       <c r="B69" s="31" t="s">
         <v>440</v>
       </c>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 00:54
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC66A40B-F00C-4F78-A3F9-4A3F9B2BCA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{199B00AC-7883-4134-A895-0662DADA300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,16 +815,154 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0000</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_0</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0002</t>
@@ -833,298 +971,160 @@
     <t>connecting solar and wind to buses in grid cell CHE_2</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
   </si>
   <si>
     <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
   </si>
   <si>
     <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E1BB19-49DC-C8BD-5D36-F42D3E7EAD4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC9840A-BABF-C400-10A5-499BA172AE21}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F327D75E-7FFF-0A86-DDD9-1C78100700B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F2B2825-6702-59DD-B89A-9BCB191EDDF4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2E4B65-4CFF-DE42-F1FB-42EEFAD01E14}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF922EA-3B45-6909-4778-600DB9CD7C0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91902494-60A6-4EDF-BB5E-BC798EBF2CCC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD1563CD-E2D8-804E-34D8-827B31B94437}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AFF12E-A44F-4DD2-A4D8-F4648BC95315}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407CF87A-FBF3-4755-98D4-BD309876A403}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF16765-DA2B-4117-8983-5F76C938EF76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B78C8B8-A88E-40B7-8BB5-AC5F3DF4E3AB}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770D557E-9C91-46EF-B281-7F4D115EC9EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DB7BC-7551-47C4-9B79-D397B31ABA87}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 01:17
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{199B00AC-7883-4134-A895-0662DADA300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5BF8B39-20A6-4681-AA1F-8540FCA06908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,18 +815,66 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0024</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_24</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0008</t>
   </si>
   <si>
@@ -839,16 +887,22 @@
     <t>connecting solar and wind to buses in grid cell CHE_5</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0013</t>
@@ -857,34 +911,10 @@
     <t>connecting solar and wind to buses in grid cell CHE_13</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0009</t>
@@ -905,10 +935,22 @@
     <t>connecting solar and wind to buses in grid cell CHE_4</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0020</t>
@@ -929,54 +971,60 @@
     <t>connecting solar and wind to buses in grid cell CHE_6</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
   </si>
   <si>
@@ -995,16 +1043,22 @@
     <t>e_r5378910-220,e_w161853746-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
   </si>
   <si>
     <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
@@ -1013,34 +1067,10 @@
     <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
@@ -1061,10 +1091,22 @@
     <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
   </si>
   <si>
     <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
@@ -1083,48 +1125,6 @@
   </si>
   <si>
     <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC9840A-BABF-C400-10A5-499BA172AE21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF1E36CD-9D5E-17CD-6737-F93E7A54CF16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F2B2825-6702-59DD-B89A-9BCB191EDDF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C2C4C0-DA44-CF6F-AE98-E04B059D905D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF922EA-3B45-6909-4778-600DB9CD7C0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFBD3587-4A3D-53F8-9EA4-E97433C0CE36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD1563CD-E2D8-804E-34D8-827B31B94437}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E320453F-D92D-375A-8B64-7AD18BE8BE66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407CF87A-FBF3-4755-98D4-BD309876A403}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52619D4-EDB2-4957-BC5D-40F0E5C22724}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B78C8B8-A88E-40B7-8BB5-AC5F3DF4E3AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E13F26-06E3-4C24-8E0E-0CA9FF4DC784}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DB7BC-7551-47C4-9B79-D397B31ABA87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6B0D13-1549-4D82-88B8-9C9C45278038}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 01:25
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5BF8B39-20A6-4681-AA1F-8540FCA06908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54F6CB1B-3B37-4C60-B313-8CE34846D041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,168 +815,204 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0010</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_10</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0022</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_22</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0000</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_0</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
   </si>
   <si>
@@ -989,142 +1025,106 @@
     <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
   </si>
   <si>
     <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1806,7 +1806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF1E36CD-9D5E-17CD-6737-F93E7A54CF16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3AD08D-5998-E15C-C737-DC7DF0239B69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1861,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C2C4C0-DA44-CF6F-AE98-E04B059D905D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D110BB5-35F1-D301-7251-81D284459508}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1916,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFBD3587-4A3D-53F8-9EA4-E97433C0CE36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A6ADC9-234E-77AF-1BAE-E16483EF04F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1971,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E320453F-D92D-375A-8B64-7AD18BE8BE66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C68F37F-18CF-CE59-C0C7-2CD937F35FD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52619D4-EDB2-4957-BC5D-40F0E5C22724}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCB35EF-1A85-4472-9A31-5CEC2182A78B}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5224,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5301,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E13F26-06E3-4C24-8E0E-0CA9FF4DC784}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCA0394-6DE2-4DF0-9692-B3A15C0CEB0A}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,7 +7624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6B0D13-1549-4D82-88B8-9C9C45278038}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E2E489-32E6-4F99-B0D5-11E2A5B37962}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 02:25
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54F6CB1B-3B37-4C60-B313-8CE34846D041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79F12A95-7C5F-41BD-91DD-937728ACE7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="441">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -815,18 +815,72 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0011</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_11</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0015</t>
   </si>
   <si>
@@ -839,10 +893,76 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0003</t>
@@ -851,132 +971,66 @@
     <t>connecting solar and wind to buses in grid cell CHE_3</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
   </si>
   <si>
@@ -995,10 +1049,76 @@
     <t>e_r7933294-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
   </si>
   <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
@@ -1007,126 +1127,6 @@
     <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
     <t>e_won-CHE_0000</t>
   </si>
   <si>
@@ -1389,9 +1389,6 @@
   </si>
   <si>
     <t>Coal + CCS</t>
-  </si>
-  <si>
-    <t>Fuel cell (distributed electricity generation)</t>
   </si>
   <si>
     <t>Gas turbine</t>
@@ -1806,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3AD08D-5998-E15C-C737-DC7DF0239B69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9C7F556-B30B-89D3-3789-4F5CCDB6C671}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D110BB5-35F1-D301-7251-81D284459508}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{232ACB95-8ED0-45D3-CAB1-42A958EE9008}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1916,7 +1913,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A6ADC9-234E-77AF-1BAE-E16483EF04F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9C96BF-BA48-6B47-8B8E-0DEB8360C762}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,7 +1968,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C68F37F-18CF-CE59-C0C7-2CD937F35FD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62AAE7BF-C93C-7665-BCE1-859D58F00F53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCB35EF-1A85-4472-9A31-5CEC2182A78B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D323E0EA-D3EB-4998-84FD-AE103C5BBDCD}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,7 +4682,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4762,7 +4759,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4839,7 +4836,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4916,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4993,7 +4990,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5301,7 +5298,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5378,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5455,7 +5452,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5532,7 +5529,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5609,7 +5606,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5686,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5763,7 +5760,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5840,7 +5837,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5917,7 +5914,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5994,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6071,7 +6068,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6148,7 +6145,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6225,7 +6222,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6302,7 +6299,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6379,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6456,7 +6453,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6533,7 +6530,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6546,7 +6543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCA0394-6DE2-4DF0-9692-B3A15C0CEB0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DE7F1E-34D5-414C-8CC2-DB25DCD0BFEE}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7624,17 +7621,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E2E489-32E6-4F99-B0D5-11E2A5B37962}">
-  <dimension ref="A1:Q69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98386404-CABD-4873-B289-BD755D36CB71}">
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="2" max="2" width="27.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="10.59765625" customWidth="1"/>
     <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="30.59765625" customWidth="1"/>
+    <col min="12" max="12" width="27.19921875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.59765625" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1"/>
@@ -7745,7 +7742,7 @@
         <v>239</v>
       </c>
       <c r="Q4" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -7787,7 +7784,7 @@
         <v>239</v>
       </c>
       <c r="Q5" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -7829,7 +7826,7 @@
         <v>239</v>
       </c>
       <c r="Q6" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -7871,7 +7868,7 @@
         <v>239</v>
       </c>
       <c r="Q7" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -7913,7 +7910,7 @@
         <v>239</v>
       </c>
       <c r="Q8" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -7955,7 +7952,7 @@
         <v>239</v>
       </c>
       <c r="Q9" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -7997,7 +7994,7 @@
         <v>239</v>
       </c>
       <c r="Q10" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -8039,7 +8036,7 @@
         <v>239</v>
       </c>
       <c r="Q11" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -8081,7 +8078,7 @@
         <v>239</v>
       </c>
       <c r="Q12" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -8123,7 +8120,7 @@
         <v>239</v>
       </c>
       <c r="Q13" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -8165,7 +8162,7 @@
         <v>239</v>
       </c>
       <c r="Q14" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -8207,7 +8204,7 @@
         <v>239</v>
       </c>
       <c r="Q15" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -8249,7 +8246,7 @@
         <v>239</v>
       </c>
       <c r="Q16" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="2:17">
@@ -8291,7 +8288,7 @@
         <v>239</v>
       </c>
       <c r="Q17" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" spans="2:17">
@@ -8333,7 +8330,7 @@
         <v>239</v>
       </c>
       <c r="Q18" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="2:17">
@@ -8375,7 +8372,7 @@
         <v>239</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="2:17">
@@ -8417,7 +8414,7 @@
         <v>239</v>
       </c>
       <c r="Q20" s="30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="2:17">
@@ -8442,25 +8439,6 @@
       <c r="H21" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="K21" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="L21" s="31" t="s">
-        <v>440</v>
-      </c>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="O21" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="P21" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q21" s="31" t="s">
-        <v>441</v>
-      </c>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="30" t="s">
@@ -8490,19 +8468,19 @@
         <v>428</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="33">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F23" s="33">
-        <v>0.54</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="G23" s="33">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
       <c r="H23" s="31" t="s">
         <v>289</v>
@@ -8513,19 +8491,19 @@
         <v>428</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="32">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="F24" s="32">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="G24" s="32">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="H24" s="30" t="s">
         <v>421</v>
@@ -8536,19 +8514,19 @@
         <v>428</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="33">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F25" s="33">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G25" s="33">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H25" s="31" t="s">
         <v>422</v>
@@ -8559,19 +8537,19 @@
         <v>429</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="32">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F26" s="32">
-        <v>0.41000000000000003</v>
+        <v>1</v>
       </c>
       <c r="G26" s="32">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="H26" s="30" t="s">
         <v>289</v>
@@ -8582,22 +8560,22 @@
         <v>429</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E27" s="33">
-        <v>500</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="F27" s="33">
-        <v>500</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="G27" s="33">
-        <v>500</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="2:17">
@@ -8605,27 +8583,27 @@
         <v>429</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="32">
-        <v>20</v>
+        <v>2650</v>
       </c>
       <c r="F28" s="32">
-        <v>20</v>
+        <v>2650</v>
       </c>
       <c r="G28" s="32">
-        <v>20</v>
+        <v>2650</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>30</v>
@@ -8634,21 +8612,21 @@
         <v>19</v>
       </c>
       <c r="E29" s="33">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="F29" s="33">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="G29" s="33">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>289</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>30</v>
@@ -8657,16 +8635,16 @@
         <v>19</v>
       </c>
       <c r="E30" s="32">
-        <v>0.35000000000000003</v>
+        <v>4</v>
       </c>
       <c r="F30" s="32">
-        <v>0.35000000000000003</v>
+        <v>4</v>
       </c>
       <c r="G30" s="32">
-        <v>0.35000000000000003</v>
+        <v>4</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="2:17">
@@ -8674,22 +8652,22 @@
         <v>430</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="33">
-        <v>2650</v>
+        <v>0.45</v>
       </c>
       <c r="F31" s="33">
-        <v>2650</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="G31" s="33">
-        <v>2650</v>
+        <v>0.5</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>421</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="2:17">
@@ -8697,22 +8675,22 @@
         <v>430</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="32">
-        <v>65</v>
+        <v>2500</v>
       </c>
       <c r="F32" s="32">
-        <v>65</v>
+        <v>2350</v>
       </c>
       <c r="G32" s="32">
-        <v>65</v>
+        <v>2300</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -8720,22 +8698,22 @@
         <v>430</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="33">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F33" s="33">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="G33" s="33">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -8743,19 +8721,19 @@
         <v>431</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="32">
-        <v>0.45</v>
+        <v>0.36</v>
       </c>
       <c r="F34" s="32">
-        <v>0.47000000000000003</v>
+        <v>0.38</v>
       </c>
       <c r="G34" s="32">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="H34" s="30" t="s">
         <v>289</v>
@@ -8766,19 +8744,19 @@
         <v>431</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="33">
-        <v>2500</v>
+        <v>5850</v>
       </c>
       <c r="F35" s="33">
-        <v>2350</v>
+        <v>5700</v>
       </c>
       <c r="G35" s="33">
-        <v>2300</v>
+        <v>5100</v>
       </c>
       <c r="H35" s="31" t="s">
         <v>421</v>
@@ -8789,19 +8767,19 @@
         <v>431</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="32">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="F36" s="32">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="G36" s="32">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="H36" s="30" t="s">
         <v>422</v>
@@ -8812,19 +8790,19 @@
         <v>432</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D37" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="33">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="F37" s="33">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="G37" s="33">
-        <v>0.43</v>
+        <v>0.33</v>
       </c>
       <c r="H37" s="31" t="s">
         <v>289</v>
@@ -8835,19 +8813,19 @@
         <v>432</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="32">
-        <v>5850</v>
+        <v>6600</v>
       </c>
       <c r="F38" s="32">
-        <v>5700</v>
+        <v>5100</v>
       </c>
       <c r="G38" s="32">
-        <v>5100</v>
+        <v>4500</v>
       </c>
       <c r="H38" s="30" t="s">
         <v>421</v>
@@ -8858,19 +8836,19 @@
         <v>432</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="33">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="F39" s="33">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="G39" s="33">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="H39" s="31" t="s">
         <v>422</v>
@@ -8881,19 +8859,19 @@
         <v>433</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="32">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="F40" s="32">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="G40" s="32">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
       <c r="H40" s="30" t="s">
         <v>289</v>
@@ -8904,19 +8882,19 @@
         <v>433</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="33">
-        <v>6600</v>
+        <v>5700</v>
       </c>
       <c r="F41" s="33">
+        <v>5700</v>
+      </c>
+      <c r="G41" s="33">
         <v>5100</v>
-      </c>
-      <c r="G41" s="33">
-        <v>4500</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>421</v>
@@ -8927,19 +8905,19 @@
         <v>433</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="32">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F42" s="32">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G42" s="32">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H42" s="30" t="s">
         <v>422</v>
@@ -8950,19 +8928,19 @@
         <v>434</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="33">
-        <v>0.37</v>
+        <v>1</v>
       </c>
       <c r="F43" s="33">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="G43" s="33">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="H43" s="31" t="s">
         <v>289</v>
@@ -8973,22 +8951,22 @@
         <v>434</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D44" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="32">
-        <v>5700</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F44" s="32">
-        <v>5700</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G44" s="32">
-        <v>5100</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -8996,27 +8974,27 @@
         <v>434</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="33">
-        <v>170</v>
+        <v>750</v>
       </c>
       <c r="F45" s="33">
-        <v>170</v>
+        <v>480</v>
       </c>
       <c r="G45" s="33">
-        <v>155</v>
+        <v>340</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="30" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C46" s="30" t="s">
         <v>28</v>
@@ -9025,21 +9003,21 @@
         <v>19</v>
       </c>
       <c r="E46" s="32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F46" s="32">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G46" s="32">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>289</v>
+        <v>422</v>
       </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C47" s="31" t="s">
         <v>28</v>
@@ -9048,16 +9026,16 @@
         <v>19</v>
       </c>
       <c r="E47" s="33">
-        <v>0.14000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="F47" s="33">
-        <v>0.14000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="G47" s="33">
-        <v>0.14000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -9065,22 +9043,22 @@
         <v>435</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="32">
-        <v>750</v>
+        <v>0.39</v>
       </c>
       <c r="F48" s="32">
-        <v>480</v>
+        <v>0.39</v>
       </c>
       <c r="G48" s="32">
-        <v>340</v>
+        <v>0.39</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>421</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="2:8">
@@ -9088,22 +9066,22 @@
         <v>435</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D49" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="33">
-        <v>12</v>
+        <v>1700</v>
       </c>
       <c r="F49" s="33">
-        <v>10</v>
+        <v>1700</v>
       </c>
       <c r="G49" s="33">
-        <v>10</v>
+        <v>1700</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="50" spans="2:8">
@@ -9111,22 +9089,22 @@
         <v>435</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D50" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="32">
-        <v>1.5</v>
+        <v>45</v>
       </c>
       <c r="F50" s="32">
-        <v>1.5</v>
+        <v>45</v>
       </c>
       <c r="G50" s="32">
-        <v>1.5</v>
+        <v>45</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="2:8">
@@ -9140,13 +9118,13 @@
         <v>19</v>
       </c>
       <c r="E51" s="33">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="F51" s="33">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="G51" s="33">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="H51" s="31" t="s">
         <v>289</v>
@@ -9163,13 +9141,13 @@
         <v>19</v>
       </c>
       <c r="E52" s="32">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="F52" s="32">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="G52" s="32">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="H52" s="30" t="s">
         <v>421</v>
@@ -9186,13 +9164,13 @@
         <v>19</v>
       </c>
       <c r="E53" s="33">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F53" s="33">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G53" s="33">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H53" s="31" t="s">
         <v>422</v>
@@ -9209,13 +9187,13 @@
         <v>19</v>
       </c>
       <c r="E54" s="32">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="F54" s="32">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="G54" s="32">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="H54" s="30" t="s">
         <v>289</v>
@@ -9232,13 +9210,13 @@
         <v>19</v>
       </c>
       <c r="E55" s="33">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="F55" s="33">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="G55" s="33">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="H55" s="31" t="s">
         <v>421</v>
@@ -9255,13 +9233,13 @@
         <v>19</v>
       </c>
       <c r="E56" s="32">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F56" s="32">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G56" s="32">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H56" s="30" t="s">
         <v>422</v>
@@ -9272,19 +9250,19 @@
         <v>438</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="33">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="F57" s="33">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="G57" s="33">
-        <v>0.48</v>
+        <v>1</v>
       </c>
       <c r="H57" s="31" t="s">
         <v>289</v>
@@ -9295,22 +9273,22 @@
         <v>438</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D58" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="32">
-        <v>2200</v>
+        <v>0.5</v>
       </c>
       <c r="F58" s="32">
-        <v>2200</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G58" s="32">
-        <v>2200</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="59" spans="2:8">
@@ -9318,27 +9296,27 @@
         <v>438</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="33">
-        <v>65</v>
+        <v>3120</v>
       </c>
       <c r="F59" s="33">
-        <v>65</v>
+        <v>2280</v>
       </c>
       <c r="G59" s="33">
-        <v>65</v>
+        <v>1660</v>
       </c>
       <c r="H59" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C60" s="30" t="s">
         <v>29</v>
@@ -9347,21 +9325,21 @@
         <v>19</v>
       </c>
       <c r="E60" s="32">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F60" s="32">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G60" s="32">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>289</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="31" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>29</v>
@@ -9370,16 +9348,16 @@
         <v>19</v>
       </c>
       <c r="E61" s="33">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F61" s="33">
-        <v>0.55000000000000004</v>
+        <v>3</v>
       </c>
       <c r="G61" s="33">
-        <v>0.56000000000000005</v>
+        <v>3</v>
       </c>
       <c r="H61" s="31" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="2:8">
@@ -9393,16 +9371,16 @@
         <v>19</v>
       </c>
       <c r="E62" s="32">
-        <v>3120</v>
+        <v>1</v>
       </c>
       <c r="F62" s="32">
-        <v>2280</v>
+        <v>1</v>
       </c>
       <c r="G62" s="32">
-        <v>1660</v>
+        <v>1</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>421</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="2:8">
@@ -9416,16 +9394,16 @@
         <v>19</v>
       </c>
       <c r="E63" s="33">
-        <v>60</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F63" s="33">
-        <v>50</v>
+        <v>0.3</v>
       </c>
       <c r="G63" s="33">
-        <v>40</v>
+        <v>0.3</v>
       </c>
       <c r="H63" s="31" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="2:8">
@@ -9439,21 +9417,21 @@
         <v>19</v>
       </c>
       <c r="E64" s="32">
-        <v>3</v>
+        <v>1630</v>
       </c>
       <c r="F64" s="32">
-        <v>3</v>
+        <v>1550</v>
       </c>
       <c r="G64" s="32">
-        <v>3</v>
+        <v>1490</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>29</v>
@@ -9462,21 +9440,21 @@
         <v>19</v>
       </c>
       <c r="E65" s="33">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F65" s="33">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="G65" s="33">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="H65" s="31" t="s">
-        <v>289</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C66" s="30" t="s">
         <v>29</v>
@@ -9485,84 +9463,15 @@
         <v>19</v>
       </c>
       <c r="E66" s="32">
-        <v>0.28999999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="F66" s="32">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="G66" s="32">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8">
-      <c r="B67" s="31" t="s">
-        <v>440</v>
-      </c>
-      <c r="C67" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D67" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="33">
-        <v>1630</v>
-      </c>
-      <c r="F67" s="33">
-        <v>1550</v>
-      </c>
-      <c r="G67" s="33">
-        <v>1490</v>
-      </c>
-      <c r="H67" s="31" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="C68" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="32">
-        <v>42</v>
-      </c>
-      <c r="F68" s="32">
-        <v>40</v>
-      </c>
-      <c r="G68" s="32">
-        <v>38</v>
-      </c>
-      <c r="H68" s="30" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" s="31" t="s">
-        <v>440</v>
-      </c>
-      <c r="C69" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E69" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="F69" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="G69" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="H69" s="31" t="s">
         <v>423</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-15 15:16
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65ABD6AC-6D8F-45C0-8A1A-2258EED263CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD5718EE-60F9-480A-B715-30BC6C42A7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,18 +815,54 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0011</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_11</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_elc_won-CHE_0015</t>
   </si>
   <si>
@@ -839,58 +875,94 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
+    <t>distr_elc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_elc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
     <t>distr_elc_won-CHE_0003</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_3</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+    <t>distr_elc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
   </si>
   <si>
     <t>distr_elc_won-CHE_0012</t>
@@ -899,84 +971,48 @@
     <t>connecting solar and wind to buses in grid cell CHE_12</t>
   </si>
   <si>
-    <t>distr_elc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_elc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
   </si>
   <si>
@@ -995,136 +1031,100 @@
     <t>e_r7933294-380</t>
   </si>
   <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
   </si>
   <si>
     <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
   </si>
   <si>
     <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1803,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C566DD03-B1C5-2CF6-A1A8-D29F3DADFF84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B8727F-0180-0104-3F5E-3BAC9C6AA042}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D01B52-9C68-5D56-1783-F62ADE50A02F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E044831-113F-F702-AA35-F58A8A06D7BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,7 +1913,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61E00438-D2D9-0679-C9A4-417492CAFE17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBDB7302-0FA1-5B59-CD8B-DC295CAD6810}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,7 +1968,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8805E7AA-D29E-4495-CCDC-79B938D9E4A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{076BAD89-C0A0-ABBE-5190-8D6FF5ECDD62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4471,7 +4471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1EFF98-EBFF-4106-B2D7-707B533714B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBD17A7-AFC1-4198-8CA4-2913CDEE3D4F}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4682,7 +4682,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4759,7 +4759,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4836,7 +4836,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4913,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4990,7 +4990,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5067,7 +5067,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5221,7 +5221,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5298,7 +5298,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5375,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5452,7 +5452,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5529,7 +5529,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5606,7 +5606,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5683,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5760,7 +5760,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5837,7 +5837,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5914,7 +5914,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5991,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6068,7 +6068,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6145,7 +6145,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6222,7 +6222,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6299,7 +6299,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6376,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6453,7 +6453,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6530,7 +6530,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -6543,7 +6543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF8269B-8EAF-4D76-BBA7-454A6782B43F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04E1105-E442-42D4-844A-18A3C6796092}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7621,7 +7621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E821221-5BCB-4AC6-932F-86654232D58F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A1826D-E338-4079-A91D-E405A37C3CD0}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-16 17:49
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8C7C6C8-97E9-47A9-A4DF-A40650B86B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE29CFAE-4821-42A5-8DF1-499FDBBB1560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>elc_buildings,elc_industry,elc_transport</t>
   </si>
   <si>
-    <t>elc_demand</t>
-  </si>
-  <si>
     <t>~FI_Comm</t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t>Car battery - 6kw/60Kwh - with V2G (optional)</t>
   </si>
   <si>
-    <t>EV_Battery</t>
-  </si>
-  <si>
     <t>elc_roadtransport</t>
   </si>
   <si>
@@ -428,6 +422,12 @@
     <t>~FI_T: USD21~FX~ACT_BND</t>
   </si>
   <si>
+    <t>ev_battery</t>
+  </si>
+  <si>
+    <t>e_demand</t>
+  </si>
+  <si>
     <t>~fi_process</t>
   </si>
   <si>
@@ -815,18 +815,114 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0024</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_24</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_solelc_won-CHE_0008</t>
   </si>
   <si>
@@ -839,82 +935,16 @@
     <t>connecting solar and wind to buses in grid cell CHE_5</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+    <t>distr_solelc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
     <t>distr_solelc_won-CHE_0012</t>
@@ -923,30 +953,6 @@
     <t>connecting solar and wind to buses in grid cell CHE_12</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
     <t>distr_solelc_won-CHE_0009</t>
   </si>
   <si>
@@ -965,18 +971,108 @@
     <t>connecting solar and wind to buses in grid cell CHE_4</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
   </si>
   <si>
@@ -995,82 +1091,16 @@
     <t>e_r5378910-220,e_w161853746-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
@@ -1079,30 +1109,6 @@
     <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
     <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
   </si>
   <si>
@@ -1119,12 +1125,6 @@
   </si>
   <si>
     <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1803,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A8E5784-0BE7-F4C5-3C33-D17A4D41FB81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFE90A40-6568-31B7-CB01-C07A1E9A75B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F55ECA2-874F-77B6-8D30-223F171D73E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4C1AF8C-633A-9EB6-313F-E38C1CCB4C76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,7 +1913,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{823F9393-DE57-4A9B-1C71-BF2F4FC002DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72DF9E42-3C51-2EA2-F33E-262F3EED6543}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,7 +1968,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E35166-367B-7711-1A18-FC16CAB116D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB81723-8901-7B1F-CCFD-C67548C9BC2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2269,7 +2269,7 @@
   <dimension ref="B2:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2336,7 +2336,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" s="1">
         <v>2022</v>
@@ -2418,7 +2418,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -2432,7 +2432,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="str">
         <f>C6</f>
-        <v>elc_demand</v>
+        <v>e_demand</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>19</v>
@@ -2450,15 +2450,15 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="T6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -2491,10 +2491,10 @@
     </row>
     <row r="8" spans="2:20">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -2508,7 +2508,7 @@
       <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -2523,10 +2523,10 @@
     </row>
     <row r="9" spans="2:20">
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -2540,7 +2540,7 @@
       <c r="I9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2565,7 +2565,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2590,7 +2590,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2615,7 +2615,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2640,7 +2640,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2665,7 +2665,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2690,7 +2690,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2715,7 +2715,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2867,7 +2867,7 @@
         <v>111</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="30" t="s">
         <v>19</v>
@@ -2901,7 +2901,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>19</v>
@@ -2935,7 +2935,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="30" t="s">
         <v>19</v>
@@ -2959,7 +2959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD6D8AA-F8A9-4BBE-94C7-C767CA3BCC03}">
   <dimension ref="B2:W61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
@@ -2987,7 +2989,7 @@
   <sheetData>
     <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2999,42 +3001,42 @@
     </row>
     <row r="3" spans="2:23">
       <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:23">
       <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="5" t="s">
@@ -3045,13 +3047,13 @@
     </row>
     <row r="5" spans="2:23">
       <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="5" t="s">
@@ -3073,7 +3075,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -3096,10 +3098,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>11</v>
@@ -3109,16 +3111,16 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="N9" s="6">
         <f>J35</f>
@@ -3152,24 +3154,24 @@
         <v>3</v>
       </c>
       <c r="V9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9" t="s">
         <v>60</v>
-      </c>
-      <c r="W9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:23">
       <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -3179,13 +3181,13 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>19</v>
@@ -3215,13 +3217,13 @@
     <row r="11" spans="2:23">
       <c r="B11" s="5"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>10</v>
@@ -3231,13 +3233,13 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>19</v>
@@ -3269,13 +3271,13 @@
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="7" t="s">
@@ -3302,10 +3304,10 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -3343,10 +3345,10 @@
     </row>
     <row r="14" spans="2:23">
       <c r="I14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4">
         <f>J44</f>
@@ -3379,10 +3381,10 @@
     </row>
     <row r="15" spans="2:23">
       <c r="I15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -3399,10 +3401,10 @@
     </row>
     <row r="16" spans="2:23">
       <c r="I16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N16" s="9">
         <v>31.536000000000001</v>
@@ -3416,10 +3418,10 @@
     </row>
     <row r="17" spans="9:23">
       <c r="I17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N17" s="4">
         <v>0.85</v>
@@ -3433,13 +3435,13 @@
     </row>
     <row r="18" spans="9:23">
       <c r="I18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>19</v>
@@ -3468,13 +3470,13 @@
     </row>
     <row r="19" spans="9:23">
       <c r="I19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" t="s">
         <v>68</v>
-      </c>
-      <c r="K19" t="s">
-        <v>69</v>
       </c>
       <c r="L19" t="s">
         <v>19</v>
@@ -3499,13 +3501,13 @@
     </row>
     <row r="20" spans="9:23">
       <c r="I20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -3522,10 +3524,10 @@
     </row>
     <row r="21" spans="9:23">
       <c r="I21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N21" s="4">
         <f>J49</f>
@@ -3558,10 +3560,10 @@
     </row>
     <row r="22" spans="9:23">
       <c r="I22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N22" s="4">
         <f>J53</f>
@@ -3594,10 +3596,10 @@
     </row>
     <row r="23" spans="9:23">
       <c r="I23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M23" t="s">
         <v>18</v>
@@ -3614,10 +3616,10 @@
     </row>
     <row r="24" spans="9:23">
       <c r="I24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N24" s="9">
         <v>31.536000000000001</v>
@@ -3631,10 +3633,10 @@
     </row>
     <row r="25" spans="9:23">
       <c r="I25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N25" s="4">
         <v>0.85</v>
@@ -3648,7 +3650,7 @@
     </row>
     <row r="31" spans="9:23" ht="15.75">
       <c r="I31" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -3660,7 +3662,7 @@
     </row>
     <row r="32" spans="9:23" ht="15.75">
       <c r="I32" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
@@ -3682,7 +3684,7 @@
     </row>
     <row r="34" spans="9:16" ht="15.75">
       <c r="I34" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -3718,7 +3720,7 @@
     </row>
     <row r="36" spans="9:16" ht="15.75">
       <c r="I36" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
@@ -3730,7 +3732,7 @@
     </row>
     <row r="37" spans="9:16" ht="15.75">
       <c r="I37" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -3742,7 +3744,7 @@
     </row>
     <row r="38" spans="9:16" ht="15.75">
       <c r="I38" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J38" s="16">
         <v>1363</v>
@@ -3768,7 +3770,7 @@
     </row>
     <row r="39" spans="9:16" ht="15.75">
       <c r="I39" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J39" s="16">
         <v>1363</v>
@@ -3794,7 +3796,7 @@
     </row>
     <row r="40" spans="9:16" ht="15.75">
       <c r="I40" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J40" s="16">
         <v>1363</v>
@@ -3820,7 +3822,7 @@
     </row>
     <row r="41" spans="9:16" ht="15.75">
       <c r="I41" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -3832,7 +3834,7 @@
     </row>
     <row r="42" spans="9:16" ht="15.75">
       <c r="I42" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J42" s="18">
         <v>34</v>
@@ -3858,7 +3860,7 @@
     </row>
     <row r="43" spans="9:16" ht="15.75">
       <c r="I43" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J43" s="18">
         <v>34</v>
@@ -3884,7 +3886,7 @@
     </row>
     <row r="44" spans="9:16" ht="15.75">
       <c r="I44" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J44" s="18">
         <v>34</v>
@@ -3910,7 +3912,7 @@
     </row>
     <row r="45" spans="9:16" ht="15.75">
       <c r="I45" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -3922,7 +3924,7 @@
     </row>
     <row r="46" spans="9:16" ht="15.75">
       <c r="I46" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -3934,7 +3936,7 @@
     </row>
     <row r="47" spans="9:16" ht="15.75">
       <c r="I47" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J47" s="16">
         <v>2470</v>
@@ -3960,7 +3962,7 @@
     </row>
     <row r="48" spans="9:16" ht="15.75">
       <c r="I48" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J48" s="16">
         <v>2470</v>
@@ -3986,7 +3988,7 @@
     </row>
     <row r="49" spans="9:16" ht="15.75">
       <c r="I49" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J49" s="16">
         <v>2470</v>
@@ -4012,7 +4014,7 @@
     </row>
     <row r="50" spans="9:16" ht="15.75">
       <c r="I50" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -4024,7 +4026,7 @@
     </row>
     <row r="51" spans="9:16" ht="15.75">
       <c r="I51" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J51" s="18">
         <v>62</v>
@@ -4050,7 +4052,7 @@
     </row>
     <row r="52" spans="9:16" ht="15.75">
       <c r="I52" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J52" s="18">
         <v>62</v>
@@ -4076,7 +4078,7 @@
     </row>
     <row r="53" spans="9:16" ht="15.75">
       <c r="I53" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J53" s="18">
         <v>62</v>
@@ -4112,7 +4114,7 @@
     </row>
     <row r="55" spans="9:16" ht="15.75">
       <c r="I55" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J55" s="11">
         <v>0.85</v>
@@ -4126,7 +4128,7 @@
     </row>
     <row r="56" spans="9:16" ht="15.75">
       <c r="I56" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
@@ -4138,7 +4140,7 @@
     </row>
     <row r="57" spans="9:16" ht="15.75">
       <c r="I57" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
@@ -4199,7 +4201,7 @@
   <dimension ref="B3:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4236,7 +4238,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -4269,16 +4271,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
       </c>
       <c r="I4">
         <v>2030</v>
@@ -4287,22 +4289,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="M4" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>93</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>94</v>
       </c>
       <c r="Q4" s="23"/>
       <c r="R4" s="23" t="s">
@@ -4315,30 +4317,30 @@
         <v>7</v>
       </c>
       <c r="U4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="V4" s="23" t="s">
-        <v>56</v>
       </c>
       <c r="W4" s="23" t="s">
         <v>11</v>
       </c>
       <c r="X4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" s="23" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="5" spans="2:25">
-      <c r="B5" s="23" t="s">
-        <v>98</v>
+      <c r="B5" t="s">
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="23">
         <v>0.90249999999999997</v>
@@ -4361,14 +4363,14 @@
       </c>
       <c r="Q5" s="23"/>
       <c r="R5" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S5" s="23" t="str">
         <f>B5</f>
-        <v>EV_Battery</v>
+        <v>ev_battery</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U5" s="23" t="s">
         <v>21</v>
@@ -4385,7 +4387,7 @@
     <row r="6" spans="2:25">
       <c r="B6" s="23"/>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="23"/>
       <c r="L6" s="24">
@@ -4408,10 +4410,10 @@
     <row r="7" spans="2:25">
       <c r="B7" s="23"/>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
@@ -4441,7 +4443,7 @@
         <v>AuxStoIN</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -4471,7 +4473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C34107-A4FA-41A2-BB44-298D61C7FCE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8ED6DB-F5DB-4406-A181-E9533E2DCBB0}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4682,7 +4684,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4759,7 +4761,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>230</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4836,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4913,7 +4915,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -4990,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5067,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5144,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5221,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5298,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5375,7 +5377,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5452,7 +5454,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5529,7 +5531,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5606,7 +5608,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5683,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5760,7 +5762,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5837,7 +5839,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5914,7 +5916,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -5991,7 +5993,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6068,7 +6070,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6299,7 +6301,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>232</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6376,7 +6378,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6453,7 +6455,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6530,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6543,7 +6545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7396BFA1-A32C-48F8-9726-6686ADC6566D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0154C7DB-E3E7-4F2B-9C87-C4BD3AFA1012}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7621,7 +7623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501058AB-0F6F-4823-A7D5-E138F8464F98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD62E59-EE38-4783-AF91-7E483830F1B6}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7679,7 +7681,7 @@
         <v>2050</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="29" t="s">
         <v>123</v>
@@ -7708,7 +7710,7 @@
         <v>419</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>19</v>
@@ -7750,7 +7752,7 @@
         <v>419</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>19</v>
@@ -7792,7 +7794,7 @@
         <v>419</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>19</v>
@@ -7834,7 +7836,7 @@
         <v>419</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>19</v>
@@ -7876,7 +7878,7 @@
         <v>419</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>19</v>
@@ -7918,7 +7920,7 @@
         <v>424</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>19</v>
@@ -7960,7 +7962,7 @@
         <v>424</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>19</v>
@@ -8002,7 +8004,7 @@
         <v>424</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>19</v>
@@ -8044,7 +8046,7 @@
         <v>424</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>19</v>
@@ -8086,7 +8088,7 @@
         <v>424</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>19</v>
@@ -8128,7 +8130,7 @@
         <v>425</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>19</v>
@@ -8170,7 +8172,7 @@
         <v>425</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>19</v>
@@ -8212,7 +8214,7 @@
         <v>425</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>19</v>
@@ -8254,7 +8256,7 @@
         <v>426</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>19</v>
@@ -8296,7 +8298,7 @@
         <v>426</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>19</v>
@@ -8338,7 +8340,7 @@
         <v>426</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>19</v>
@@ -8380,7 +8382,7 @@
         <v>427</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>19</v>
@@ -8422,7 +8424,7 @@
         <v>427</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>19</v>
@@ -8445,7 +8447,7 @@
         <v>427</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>19</v>
@@ -8468,7 +8470,7 @@
         <v>428</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>19</v>
@@ -8491,7 +8493,7 @@
         <v>428</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>19</v>
@@ -8514,7 +8516,7 @@
         <v>428</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>19</v>
@@ -8537,7 +8539,7 @@
         <v>429</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>19</v>
@@ -8560,7 +8562,7 @@
         <v>429</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>19</v>
@@ -8583,7 +8585,7 @@
         <v>429</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>19</v>
@@ -8606,7 +8608,7 @@
         <v>429</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>19</v>
@@ -8629,7 +8631,7 @@
         <v>429</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>19</v>
@@ -8652,7 +8654,7 @@
         <v>430</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>19</v>
@@ -8675,7 +8677,7 @@
         <v>430</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>19</v>
@@ -8698,7 +8700,7 @@
         <v>430</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>19</v>
@@ -8721,7 +8723,7 @@
         <v>431</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>19</v>
@@ -8744,7 +8746,7 @@
         <v>431</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>19</v>
@@ -8767,7 +8769,7 @@
         <v>431</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>19</v>
@@ -8790,7 +8792,7 @@
         <v>432</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="31" t="s">
         <v>19</v>
@@ -8813,7 +8815,7 @@
         <v>432</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>19</v>
@@ -8836,7 +8838,7 @@
         <v>432</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>19</v>
@@ -8859,7 +8861,7 @@
         <v>433</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>19</v>
@@ -8882,7 +8884,7 @@
         <v>433</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>19</v>
@@ -8905,7 +8907,7 @@
         <v>433</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>19</v>
@@ -8928,7 +8930,7 @@
         <v>434</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>19</v>
@@ -8951,7 +8953,7 @@
         <v>434</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="30" t="s">
         <v>19</v>
@@ -8974,7 +8976,7 @@
         <v>434</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>19</v>
@@ -8997,7 +8999,7 @@
         <v>434</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>19</v>
@@ -9020,7 +9022,7 @@
         <v>434</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>19</v>
@@ -9043,7 +9045,7 @@
         <v>435</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>19</v>
@@ -9066,7 +9068,7 @@
         <v>435</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" s="31" t="s">
         <v>19</v>
@@ -9089,7 +9091,7 @@
         <v>435</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="30" t="s">
         <v>19</v>
@@ -9112,7 +9114,7 @@
         <v>436</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>19</v>
@@ -9135,7 +9137,7 @@
         <v>436</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>19</v>
@@ -9158,7 +9160,7 @@
         <v>436</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="31" t="s">
         <v>19</v>
@@ -9181,7 +9183,7 @@
         <v>437</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" s="30" t="s">
         <v>19</v>
@@ -9204,7 +9206,7 @@
         <v>437</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="31" t="s">
         <v>19</v>
@@ -9227,7 +9229,7 @@
         <v>437</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>19</v>
@@ -9250,7 +9252,7 @@
         <v>438</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>19</v>
@@ -9273,7 +9275,7 @@
         <v>438</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" s="30" t="s">
         <v>19</v>
@@ -9296,7 +9298,7 @@
         <v>438</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>19</v>
@@ -9319,7 +9321,7 @@
         <v>438</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D60" s="30" t="s">
         <v>19</v>
@@ -9342,7 +9344,7 @@
         <v>438</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D61" s="31" t="s">
         <v>19</v>
@@ -9365,7 +9367,7 @@
         <v>439</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D62" s="30" t="s">
         <v>19</v>
@@ -9388,7 +9390,7 @@
         <v>439</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D63" s="31" t="s">
         <v>19</v>
@@ -9411,7 +9413,7 @@
         <v>439</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D64" s="30" t="s">
         <v>19</v>
@@ -9434,7 +9436,7 @@
         <v>439</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D65" s="31" t="s">
         <v>19</v>
@@ -9457,7 +9459,7 @@
         <v>439</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D66" s="30" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-16 23:26
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A90BA0DE-6D66-4AB6-9645-7EB93A106141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25560406-F984-48FD-824B-92FEF339AA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -824,16 +824,112 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0007</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_7</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
+    <t>distr_solelc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
   </si>
   <si>
     <t>distr_solelc_won-CHE_0017</t>
@@ -854,28 +950,16 @@
     <t>connecting solar and wind to buses in grid cell CHE_23</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+    <t>distr_solelc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
     <t>distr_solelc_won-CHE_0011</t>
@@ -896,102 +980,114 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
   </si>
   <si>
     <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
   </si>
   <si>
@@ -1010,28 +1106,16 @@
     <t>e_w207991759-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
   </si>
   <si>
     <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
@@ -1050,90 +1134,6 @@
   </si>
   <si>
     <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -1812,7 +1812,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6AFDBFC-7BCF-9067-A031-261E92AFA27E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B288C5D-3B52-391B-12D0-120F972F9A49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1867,7 +1867,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{342F83EA-D4E1-0510-3B91-74C2E7E84271}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{717F4B73-04E1-0CCB-77F1-01BD193997AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1922,7 +1922,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD5C67A-ECF3-4980-BFB9-76950663E0E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C4F272C-C86F-C255-1287-C1C96AFA2C5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1977,7 +1977,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749CEB6E-F5E1-41BF-45C1-B6D0D02C50B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A4AD8B-ABBC-2000-83E2-8F4179F2EC40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4504,7 +4504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C4D652-115A-4D11-B8F2-8A2BA7B65651}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4ED5E85-7921-4676-96A2-97105CCDC909}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4715,7 +4715,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -4792,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -4869,7 +4869,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -4946,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -5023,7 +5023,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5100,7 +5100,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5177,7 +5177,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5254,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5331,7 +5331,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5408,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5485,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -5562,7 +5562,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -5716,7 +5716,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -5793,7 +5793,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -5870,7 +5870,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -5947,7 +5947,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -6024,7 +6024,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6101,7 +6101,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6178,7 +6178,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6409,7 +6409,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6486,7 +6486,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -6563,7 +6563,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -6576,7 +6576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69BBE45-8FED-49B5-9208-305B629253A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A10511-67EC-4077-B90D-E5D392B2B18A}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7654,7 +7654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBAFE67-9F65-4980-8DF0-8EFE2633AC07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309EC6CE-6A83-4BEC-B1D2-A36C10ACA654}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-18 23:58
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{779083A1-D861-4E41-AB8E-264A1F398B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17865D7C-E509-40A4-9419-07431C238D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,18 +825,54 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_14</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0018</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_18</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_9</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_21</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0004</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_4</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0011</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_11</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_solelc_won-CHE_0015</t>
   </si>
   <si>
@@ -849,144 +885,144 @@
     <t>connecting solar and wind to buses in grid cell CHE_25</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_13</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0003</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_3</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_9</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_21</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0004</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_4</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_13</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_14</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0018</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_18</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
-  </si>
-  <si>
     <t>distr_solelc_won-CHE_0012</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_12</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
+  </si>
+  <si>
+    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
+  </si>
+  <si>
+    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
+  </si>
+  <si>
+    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
+  </si>
+  <si>
+    <t>e_CH17-380,e_w211907009-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
+  </si>
+  <si>
+    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
   </si>
   <si>
@@ -1005,136 +1041,100 @@
     <t>e_r7933294-380</t>
   </si>
   <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
+  </si>
+  <si>
+    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
   </si>
   <si>
     <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
   </si>
   <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
-  </si>
-  <si>
-    <t>e_CH14-220,e_CH14-380,e_w1105061707-220,e_w1105061707-380,e_w147557680-220,e_w165254212-220,e_w402053379-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0021,elc_spv-CHE_0021</t>
-  </si>
-  <si>
-    <t>e_CH17-380,e_w211907009-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0004,elc_spv-CHE_0004</t>
-  </si>
-  <si>
-    <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
-  </si>
-  <si>
-    <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
-  </si>
-  <si>
-    <t>e_CH1-220,e_CH2-220,e_CH5-220,e_CH7-220,e_w108257952-220,e_w1284913429-220,e_w165513396-220,e_w165513396-380,e_w190819048-220,e_w27107779-220,e_w31308888-220,e_w33271433-220,e_w356292116-220,e_w356292116-380,e_w35840165-380,e_w50319857-220,e_w50319857-380,e_w50319857-400,e_w89405664-220,e_w89977424-220,e_w98648381-220,e_w98648381-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0018,elc_spv-CHE_0018</t>
-  </si>
-  <si>
-    <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
-  </si>
-  <si>
     <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
   </si>
   <si>
     <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -2251,7 +2251,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64857231-98B8-ED6E-3752-C9426713311A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78EC20C-7CEF-89BE-50A2-7C1360B9BF23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,7 +2306,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D184C502-1BAB-A9B1-2215-BE69F4DB0281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336B81FC-28C5-1EFA-3C8B-35B17523B018}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2361,7 +2361,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08F4559-A6C7-A0F4-77A8-18E75FDB56E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BBE32B9-F571-68BB-1FCE-DCDECB6C70A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2416,7 +2416,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D2393EF-A85F-DC02-69B3-9072C063C995}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4128AE72-03E5-5BD5-D026-A0E4E56D36CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,7 +2471,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B882375E-0EB1-7787-CF8A-3F6214D65397}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBBC1640-A161-6D4A-F38E-1827AC56C603}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4998,7 +4998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACC38AE-28C9-4012-B7F8-9F8B41E49F38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303AEFDB-4839-49C2-A54C-7AD44DCB24C1}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -5286,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -5363,7 +5363,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -5440,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -5517,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5671,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5748,7 +5748,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5902,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5979,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -6056,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -6133,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -6210,7 +6210,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -6287,7 +6287,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -6364,7 +6364,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -6441,7 +6441,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -6518,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6595,7 +6595,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6749,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6826,7 +6826,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6903,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6980,7 +6980,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -7057,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -7070,7 +7070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59567881-B722-44AC-9F6F-B0D7A4614F90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45435668-DD89-41BD-82D7-05E5AE2444F2}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8148,7 +8148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3637757-48F6-4CAC-938D-C8F140B954DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3532A06D-4648-4647-B96B-25B72647B59C}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10014,7 +10014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F780538-F606-49CA-8E0E-8A319ACC4F3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF19048-875F-4B07-9A8B-6647D4E6FF79}">
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -10505,7 +10505,7 @@
         <v>481</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-19 00:07
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17865D7C-E509-40A4-9419-07431C238D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A50801B-DECA-4605-9B12-294A9C386203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,24 +825,114 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0003</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_3</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0000</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_0</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0002</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_2</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_17</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0019</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_19</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0023</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_23</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0010</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_10</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_22</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_24</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0008</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_8</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_5</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_11</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_15</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_25</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0014</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_14</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_solelc_won-CHE_0018</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell CHE_18</t>
   </si>
   <si>
+    <t>distr_solelc_won-CHE_0007</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+  </si>
+  <si>
     <t>distr_solelc_won-CHE_0009</t>
   </si>
   <si>
@@ -861,70 +951,28 @@
     <t>connecting solar and wind to buses in grid cell CHE_4</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0000</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_0</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_11</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_15</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_25</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0002</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_2</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0010</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_10</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_22</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_17</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0019</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_19</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0023</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_23</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0007</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_7</t>
+    <t>distr_solelc_won-CHE_0012</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_12</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_20</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0001</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_1</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-CHE_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell CHE_6</t>
   </si>
   <si>
     <t>distr_solelc_won-CHE_0013</t>
@@ -933,60 +981,96 @@
     <t>connecting solar and wind to buses in grid cell CHE_13</t>
   </si>
   <si>
-    <t>distr_solelc_won-CHE_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_20</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0001</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_1</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_6</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_24</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0008</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_8</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_5</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0003</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_3</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-CHE_0012</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell CHE_12</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
     <t>efficiency</t>
   </si>
   <si>
+    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
+  </si>
+  <si>
+    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
+  </si>
+  <si>
+    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
+  </si>
+  <si>
+    <t>e_w232662311-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
+  </si>
+  <si>
+    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
+  </si>
+  <si>
+    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
+  </si>
+  <si>
+    <t>e_w207991759-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
+  </si>
+  <si>
+    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
+  </si>
+  <si>
+    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
+  </si>
+  <si>
+    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
+  </si>
+  <si>
+    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
+  </si>
+  <si>
+    <t>e_r5378910-220,e_w161853746-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
+  </si>
+  <si>
+    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
+  </si>
+  <si>
+    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
+  </si>
+  <si>
+    <t>e_r7933294-380</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0014,elc_spv-CHE_0014</t>
   </si>
   <si>
@@ -999,6 +1083,12 @@
     <t>e_CH3-220,e_CH6-220,e_r9310861-220,e_w11282314-220,e_w147714395-220,e_w147714395-380,e_w148015471-220,e_w22899676-220,e_w240575085-220,e_w26843160-220,e_w281809991-220,e_w50561341-220,e_w87281514-220</t>
   </si>
   <si>
+    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
+  </si>
+  <si>
+    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+  </si>
+  <si>
     <t>elc_won-CHE_0009,elc_spv-CHE_0009</t>
   </si>
   <si>
@@ -1017,124 +1107,34 @@
     <t>e_w111162936-220,e_w111162936-380,e_w111162936-400,e_w122720993-220,e_w194258388-220</t>
   </si>
   <si>
-    <t>elc_won-CHE_0000,elc_spv-CHE_0000</t>
-  </si>
-  <si>
-    <t>e_CH51-220,e_CH51-225,e_CH51-400,e_CH52-220,e_CH57-220,e_CH57-225,e_w177392130-220,e_w177392130-400,e_w239937062-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0011,elc_spv-CHE_0011</t>
-  </si>
-  <si>
-    <t>e_CH46-220,e_CH47-220,e_w228003081-220,e_w391576135-220,e_w391577741-220,e_w969819301-220,e_w969819301-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0015,elc_spv-CHE_0015</t>
-  </si>
-  <si>
-    <t>e_CH50-220,e_CH56-220,e_CH58-220,e_CH59-220,e_w1327084723-220,e_w281800404-220,e_w281803398-220,e_w281815404-220,e_w35487135-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0025,elc_spv-CHE_0025</t>
-  </si>
-  <si>
-    <t>e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0002,elc_spv-CHE_0002</t>
-  </si>
-  <si>
-    <t>e_w232662311-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0010,elc_spv-CHE_0010</t>
-  </si>
-  <si>
-    <t>e_CH11-220,e_w109037817-220,e_w109037817-380,e_w127004407-380,e_w127004407-400,e_w27435934-220,e_w30350721-220,e_w397960460-380,e_w397960460-400,e_w88901626-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0022,elc_spv-CHE_0022</t>
-  </si>
-  <si>
-    <t>e_CH4-220,e_CH9-220,e_w455120191-220,e_w83861269-220,e_w92798668-220,e_w92873516-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0017,elc_spv-CHE_0017</t>
-  </si>
-  <si>
-    <t>e_CH12-220,e_CH12-380,e_CH13-220,e_CH16-380,e_CH18-220,e_CH18-380,e_w192677427-220,e_w192677427-380,e_w52738225-220,e_w52738225-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0019,elc_spv-CHE_0019</t>
-  </si>
-  <si>
-    <t>e_CH45-220,e_w281804158-220,e_w281804158-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0023,elc_spv-CHE_0023</t>
-  </si>
-  <si>
-    <t>e_w207991759-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0007,elc_spv-CHE_0007</t>
-  </si>
-  <si>
-    <t>e_CH44-220,e_w212722603-220,e_w212722603-380,e_w236819191-220,e_w758943072-220</t>
+    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
+  </si>
+  <si>
+    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
+  </si>
+  <si>
+    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
+  </si>
+  <si>
+    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
+  </si>
+  <si>
+    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
+  </si>
+  <si>
+    <t>e_w127004407-400</t>
   </si>
   <si>
     <t>elc_won-CHE_0013,elc_spv-CHE_0013</t>
   </si>
   <si>
     <t>e_CH15-220,e_w146225999-220,e_w159527493-220,e_w242269161-220,e_w281799252-220,e_w35002638-220,e_w35002638-380,e_w97941869-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0020,elc_spv-CHE_0020</t>
-  </si>
-  <si>
-    <t>e_CH21-220,e_CH22-220,e_CH22-380,e_CH29-220,e_CH29-380,e_CH41-380,e_w1208713169-220,e_w207993342-220,e_w207993342-380,e_w208780268-380,e_w212498548-220,e_w36348118-220,e_w365556107-220,e_w71500123-220,e_w71500123-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0001,elc_spv-CHE_0001</t>
-  </si>
-  <si>
-    <t>e_CH31-220,e_w132373704-220,e_w232662311-220,e_w44496892-220,e_w55695765-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0006,elc_spv-CHE_0006</t>
-  </si>
-  <si>
-    <t>e_w127004407-400</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0024,elc_spv-CHE_0024</t>
-  </si>
-  <si>
-    <t>e_CH30-380,e_CH33-380,e_CH37-380,e_r7933294-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0008,elc_spv-CHE_0008</t>
-  </si>
-  <si>
-    <t>e_CH43-220,e_w209324991-220,e_w26166640-220,e_w402055336-220,e_w758315582-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0005,elc_spv-CHE_0005</t>
-  </si>
-  <si>
-    <t>e_r5378910-220,e_w161853746-220</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0003,elc_spv-CHE_0003</t>
-  </si>
-  <si>
-    <t>e_CH48-225,e_CH49-225,e_CH53-225,e_CH60-225,e_w234983117-220,e_w234983117-380,e_w238138373-380,e_w260211728-225,e_w260211728-380,e_w55698557-220,e_w55698557-225,e_w802058337-220,e_w802058337-225,e_w936521586-380</t>
-  </si>
-  <si>
-    <t>elc_won-CHE_0012,elc_spv-CHE_0012</t>
-  </si>
-  <si>
-    <t>e_CH19-220,e_CH20-220,e_CH25-220,e_CH27-220,e_CH34-220,e_CH34-380,e_CH35-220,e_CH36-220,e_CH38-220,e_CH39-220,e_CH40-220,e_w1086214433-220,e_w1092884227-220,e_w240959264-220,e_w364949845-220,e_w364949845-380</t>
   </si>
   <si>
     <t>e_won-CHE_0000</t>
@@ -2251,7 +2251,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78EC20C-7CEF-89BE-50A2-7C1360B9BF23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{885C1C4C-4C6A-D1E0-56BB-5A546028FEB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,7 +2306,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336B81FC-28C5-1EFA-3C8B-35B17523B018}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE9C5B7-D256-0A68-A732-FE24BD5C7105}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2361,7 +2361,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BBE32B9-F571-68BB-1FCE-DCDECB6C70A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C70A599-584D-96C9-2BA2-78F301CE690C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2416,7 +2416,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4128AE72-03E5-5BD5-D026-A0E4E56D36CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C15C12-1022-A8DF-FA5A-117DE6FF3609}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,7 +2471,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBBC1640-A161-6D4A-F38E-1827AC56C603}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69FA455F-C937-E5A5-3202-5B5A0E7A349F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4998,7 +4998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303AEFDB-4839-49C2-A54C-7AD44DCB24C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D47CC9C-8754-4385-BE05-3F017B43397B}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="30" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -5286,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="31" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -5363,7 +5363,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="30" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -5440,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -5517,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="31" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -5671,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -5748,7 +5748,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="31" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -5902,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="31" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -5979,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -6056,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="31" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -6133,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -6210,7 +6210,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -6287,7 +6287,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -6364,7 +6364,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="31" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -6441,7 +6441,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -6518,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -6595,7 +6595,7 @@
         <v>1</v>
       </c>
       <c r="AG22" s="30" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="31" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -6749,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -6826,7 +6826,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -6903,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:33">
@@ -6980,7 +6980,7 @@
         <v>1</v>
       </c>
       <c r="AG27" s="31" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -7057,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -7070,7 +7070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45435668-DD89-41BD-82D7-05E5AE2444F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F254A4-6A1B-4590-8367-3C0E2DA621D9}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8148,7 +8148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3532A06D-4648-4647-B96B-25B72647B59C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6BE372-B7BB-483A-A06E-C0FA5F62E40F}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10014,7 +10014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF19048-875F-4B07-9A8B-6647D4E6FF79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B189DDA6-F6B0-49F3-8EFD-9C081A71FAA9}">
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -10505,7 +10505,7 @@
         <v>481</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>482</v>

</xml_diff>